<commit_message>
Adding CCES 2015 Data
Adding CCES 2015 Data
Updated Variable_index with 2015 information
</commit_message>
<xml_diff>
--- a/Variable_Index.xlsx
+++ b/Variable_Index.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\dkrei\OneDrive\tempschool\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Owner\OneDrive\tempschool\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="299" documentId="8_{5BB726C6-045A-4B74-832F-0E45B46FDC8E}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{82F00D0E-7AD1-4926-9643-4CF861DD7334}"/>
+  <xr:revisionPtr revIDLastSave="492" documentId="8_{5BB726C6-045A-4B74-832F-0E45B46FDC8E}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{F41D8518-C3E8-4AF1-BF7A-9BCA7FE6CE58}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="13800" windowHeight="4416" xr2:uid="{B1787686-8DD4-4EAF-A6DB-220586B0E0A3}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="13800" windowHeight="4410" xr2:uid="{B1787686-8DD4-4EAF-A6DB-220586B0E0A3}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="235" uniqueCount="189">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="382" uniqueCount="266">
   <si>
     <t>ID</t>
   </si>
@@ -598,6 +598,237 @@
   </si>
   <si>
     <t>ccesmodule_16</t>
+  </si>
+  <si>
+    <t>weight</t>
+  </si>
+  <si>
+    <t>CC15_320a</t>
+  </si>
+  <si>
+    <t>CC15_320b</t>
+  </si>
+  <si>
+    <t>CC15_320c</t>
+  </si>
+  <si>
+    <t>CC15_320d</t>
+  </si>
+  <si>
+    <t>CC15_321_1</t>
+  </si>
+  <si>
+    <t>CC15_321_2</t>
+  </si>
+  <si>
+    <t>CC15_321_3</t>
+  </si>
+  <si>
+    <t>CC15_321_4</t>
+  </si>
+  <si>
+    <t>CC15_321_5</t>
+  </si>
+  <si>
+    <t>CC15_321_6</t>
+  </si>
+  <si>
+    <t>CC15_322a</t>
+  </si>
+  <si>
+    <t>CC15_322b</t>
+  </si>
+  <si>
+    <t>CC15_322c</t>
+  </si>
+  <si>
+    <t>CC15_322d</t>
+  </si>
+  <si>
+    <t>CC15_322e</t>
+  </si>
+  <si>
+    <t>CC15_322f</t>
+  </si>
+  <si>
+    <t>CC15_325</t>
+  </si>
+  <si>
+    <t>CC15_350</t>
+  </si>
+  <si>
+    <t>employ</t>
+  </si>
+  <si>
+    <t>pid7</t>
+  </si>
+  <si>
+    <t>milstat_5</t>
+  </si>
+  <si>
+    <t>union</t>
+  </si>
+  <si>
+    <t>starttime</t>
+  </si>
+  <si>
+    <t>endtime</t>
+  </si>
+  <si>
+    <t>Allow police to question anyone they think may be in the country illegally.</t>
+  </si>
+  <si>
+    <t>Do you favor or oppose allowing gays and lesbians to marry legally?</t>
+  </si>
+  <si>
+    <t>With which party, if any, are you registered?</t>
+  </si>
+  <si>
+    <t>Neither myself nor any members of my</t>
+  </si>
+  <si>
+    <t>V101_15</t>
+  </si>
+  <si>
+    <t>Zipcode_15</t>
+  </si>
+  <si>
+    <t>State_15</t>
+  </si>
+  <si>
+    <t>CountyFips_15</t>
+  </si>
+  <si>
+    <t>CountyName_15</t>
+  </si>
+  <si>
+    <t>Birth Year_15</t>
+  </si>
+  <si>
+    <t>Gender_15</t>
+  </si>
+  <si>
+    <t>Education_15</t>
+  </si>
+  <si>
+    <t>Race_15</t>
+  </si>
+  <si>
+    <t>Marrital Status_15</t>
+  </si>
+  <si>
+    <t>Children &lt; 18 yrs_15</t>
+  </si>
+  <si>
+    <t>Family Income_15</t>
+  </si>
+  <si>
+    <t>Employment Status_15</t>
+  </si>
+  <si>
+    <t>Own Home_15</t>
+  </si>
+  <si>
+    <t>Political Preference_15</t>
+  </si>
+  <si>
+    <t>Political Viewpoint_15</t>
+  </si>
+  <si>
+    <t>Gun Background Checks_15</t>
+  </si>
+  <si>
+    <t>Prohibit Publication_15</t>
+  </si>
+  <si>
+    <t>Ban Assult Weapons_15</t>
+  </si>
+  <si>
+    <t>Make CCP Easier_15</t>
+  </si>
+  <si>
+    <t>Grant Legal Status_15</t>
+  </si>
+  <si>
+    <t>Increase Border Patrols_15</t>
+  </si>
+  <si>
+    <t>Fine employers_15</t>
+  </si>
+  <si>
+    <t>Increase Work Visas_15</t>
+  </si>
+  <si>
+    <t>Identify and deport_15</t>
+  </si>
+  <si>
+    <t>Always Allow Choice_15</t>
+  </si>
+  <si>
+    <t>Rape, Incest, or Health_15</t>
+  </si>
+  <si>
+    <t>Prohibit &gt; 20 Weeks_15</t>
+  </si>
+  <si>
+    <t>Employers decline benefits_15</t>
+  </si>
+  <si>
+    <t>Prohibit Fed Funds_15</t>
+  </si>
+  <si>
+    <t>Illegal in all circumstances_15</t>
+  </si>
+  <si>
+    <t>Gay Marriage_15</t>
+  </si>
+  <si>
+    <t>Bornagain_15</t>
+  </si>
+  <si>
+    <t>Religious Importance_15</t>
+  </si>
+  <si>
+    <t>Church Attendance_15</t>
+  </si>
+  <si>
+    <t>Prayer Frequency_15</t>
+  </si>
+  <si>
+    <t>Religion Donomination_15</t>
+  </si>
+  <si>
+    <t>Military - I am_15</t>
+  </si>
+  <si>
+    <t>Military - Family_15</t>
+  </si>
+  <si>
+    <t>Military - I served_15</t>
+  </si>
+  <si>
+    <t>Military - Family served_15</t>
+  </si>
+  <si>
+    <t>Union - Self_15</t>
+  </si>
+  <si>
+    <t>Union - Family_15</t>
+  </si>
+  <si>
+    <t>starttime_pre_15</t>
+  </si>
+  <si>
+    <t>endtime_pre_15</t>
+  </si>
+  <si>
+    <t>commonweight_15</t>
+  </si>
+  <si>
+    <t>ccesmodule_15</t>
+  </si>
+  <si>
+    <t>CCES_2015</t>
   </si>
 </sst>
 </file>
@@ -621,12 +852,24 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="2">
+  <fills count="4">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="2" tint="-0.499984740745262"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.39997558519241921"/>
+        <bgColor indexed="64"/>
+      </patternFill>
     </fill>
   </fills>
   <borders count="1">
@@ -641,9 +884,18 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="7">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -986,26 +1238,35 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8B0C4685-FCD9-4520-9F28-50A98CF8260A}">
-  <dimension ref="B1:E61"/>
+  <dimension ref="B1:R63"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A48" workbookViewId="0">
-      <selection activeCell="D61" sqref="D2:D61"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="J1" sqref="J1:J1048576"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="2" max="2" width="12.5546875" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="24.5546875" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="42.5546875" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="141.88671875" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="12.5703125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="24.5703125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="42.5703125" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="49.5703125" style="4" customWidth="1"/>
+    <col min="6" max="6" width="2" style="2" customWidth="1"/>
+    <col min="7" max="7" width="14.85546875" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="28.7109375" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="39.140625" style="4" customWidth="1"/>
+    <col min="10" max="10" width="2" style="2" customWidth="1"/>
+    <col min="12" max="12" width="14.85546875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="2:5" x14ac:dyDescent="0.3">
+    <row r="1" spans="2:10" x14ac:dyDescent="0.25">
       <c r="C1" t="s">
         <v>32</v>
       </c>
-    </row>
-    <row r="2" spans="2:5" s="1" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="G1" t="s">
+        <v>265</v>
+      </c>
+    </row>
+    <row r="2" spans="2:10" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B2" s="1" t="s">
         <v>34</v>
       </c>
@@ -1015,12 +1276,23 @@
       <c r="D2" s="1" t="s">
         <v>36</v>
       </c>
-      <c r="E2" s="1" t="s">
+      <c r="E2" s="5" t="s">
         <v>33</v>
       </c>
-    </row>
-    <row r="3" spans="2:5" x14ac:dyDescent="0.3">
-      <c r="B3" t="s">
+      <c r="F2" s="3"/>
+      <c r="G2" s="1" t="s">
+        <v>35</v>
+      </c>
+      <c r="H2" s="1" t="s">
+        <v>36</v>
+      </c>
+      <c r="I2" s="5" t="s">
+        <v>33</v>
+      </c>
+      <c r="J2" s="3"/>
+    </row>
+    <row r="3" spans="2:10" x14ac:dyDescent="0.25">
+      <c r="B3" s="6" t="s">
         <v>0</v>
       </c>
       <c r="C3" t="s">
@@ -1029,12 +1301,21 @@
       <c r="D3" t="s">
         <v>130</v>
       </c>
-      <c r="E3" t="s">
+      <c r="E3" s="4" t="s">
         <v>105</v>
       </c>
-    </row>
-    <row r="4" spans="2:5" x14ac:dyDescent="0.3">
-      <c r="B4" t="s">
+      <c r="G3" t="s">
+        <v>1</v>
+      </c>
+      <c r="H3" t="s">
+        <v>218</v>
+      </c>
+      <c r="I3" s="4" t="s">
+        <v>105</v>
+      </c>
+    </row>
+    <row r="4" spans="2:10" x14ac:dyDescent="0.25">
+      <c r="B4" s="6" t="s">
         <v>2</v>
       </c>
       <c r="C4" t="s">
@@ -1043,12 +1324,21 @@
       <c r="D4" t="s">
         <v>131</v>
       </c>
-      <c r="E4" t="s">
+      <c r="E4" s="4" t="s">
         <v>106</v>
       </c>
-    </row>
-    <row r="5" spans="2:5" x14ac:dyDescent="0.3">
-      <c r="B5" t="s">
+      <c r="G4" t="s">
+        <v>3</v>
+      </c>
+      <c r="H4" t="s">
+        <v>219</v>
+      </c>
+      <c r="I4" s="4" t="s">
+        <v>106</v>
+      </c>
+    </row>
+    <row r="5" spans="2:10" x14ac:dyDescent="0.25">
+      <c r="B5" s="6" t="s">
         <v>2</v>
       </c>
       <c r="C5" t="s">
@@ -1057,12 +1347,21 @@
       <c r="D5" t="s">
         <v>132</v>
       </c>
-      <c r="E5" t="s">
+      <c r="E5" s="4" t="s">
         <v>107</v>
       </c>
-    </row>
-    <row r="6" spans="2:5" x14ac:dyDescent="0.3">
-      <c r="B6" t="s">
+      <c r="G5" t="s">
+        <v>4</v>
+      </c>
+      <c r="H5" t="s">
+        <v>220</v>
+      </c>
+      <c r="I5" s="4" t="s">
+        <v>107</v>
+      </c>
+    </row>
+    <row r="6" spans="2:10" x14ac:dyDescent="0.25">
+      <c r="B6" s="6" t="s">
         <v>2</v>
       </c>
       <c r="C6" t="s">
@@ -1071,12 +1370,21 @@
       <c r="D6" t="s">
         <v>133</v>
       </c>
-      <c r="E6" t="s">
+      <c r="E6" s="4" t="s">
         <v>108</v>
       </c>
-    </row>
-    <row r="7" spans="2:5" x14ac:dyDescent="0.3">
-      <c r="B7" t="s">
+      <c r="G6" t="s">
+        <v>5</v>
+      </c>
+      <c r="H6" t="s">
+        <v>221</v>
+      </c>
+      <c r="I6" s="4" t="s">
+        <v>108</v>
+      </c>
+    </row>
+    <row r="7" spans="2:10" x14ac:dyDescent="0.25">
+      <c r="B7" s="6" t="s">
         <v>2</v>
       </c>
       <c r="C7" t="s">
@@ -1085,12 +1393,21 @@
       <c r="D7" t="s">
         <v>134</v>
       </c>
-      <c r="E7" t="s">
+      <c r="E7" s="4" t="s">
         <v>109</v>
       </c>
-    </row>
-    <row r="8" spans="2:5" x14ac:dyDescent="0.3">
-      <c r="B8" t="s">
+      <c r="G7" t="s">
+        <v>6</v>
+      </c>
+      <c r="H7" t="s">
+        <v>222</v>
+      </c>
+      <c r="I7" s="4" t="s">
+        <v>109</v>
+      </c>
+    </row>
+    <row r="8" spans="2:10" x14ac:dyDescent="0.25">
+      <c r="B8" s="6" t="s">
         <v>7</v>
       </c>
       <c r="C8" t="s">
@@ -1099,12 +1416,21 @@
       <c r="D8" t="s">
         <v>135</v>
       </c>
-      <c r="E8" t="s">
+      <c r="E8" s="4" t="s">
         <v>71</v>
       </c>
-    </row>
-    <row r="9" spans="2:5" x14ac:dyDescent="0.3">
-      <c r="B9" t="s">
+      <c r="G8" t="s">
+        <v>8</v>
+      </c>
+      <c r="H8" t="s">
+        <v>223</v>
+      </c>
+      <c r="I8" s="4" t="s">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="9" spans="2:10" x14ac:dyDescent="0.25">
+      <c r="B9" s="6" t="s">
         <v>7</v>
       </c>
       <c r="C9" t="s">
@@ -1113,12 +1439,21 @@
       <c r="D9" t="s">
         <v>136</v>
       </c>
-      <c r="E9" t="s">
+      <c r="E9" s="4" t="s">
         <v>72</v>
       </c>
-    </row>
-    <row r="10" spans="2:5" x14ac:dyDescent="0.3">
-      <c r="B10" t="s">
+      <c r="G9" t="s">
+        <v>9</v>
+      </c>
+      <c r="H9" t="s">
+        <v>224</v>
+      </c>
+      <c r="I9" s="4" t="s">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="10" spans="2:10" x14ac:dyDescent="0.25">
+      <c r="B10" s="6" t="s">
         <v>7</v>
       </c>
       <c r="C10" t="s">
@@ -1127,12 +1462,21 @@
       <c r="D10" t="s">
         <v>137</v>
       </c>
-      <c r="E10" t="s">
+      <c r="E10" s="4" t="s">
         <v>73</v>
       </c>
-    </row>
-    <row r="11" spans="2:5" x14ac:dyDescent="0.3">
-      <c r="B11" t="s">
+      <c r="G10" t="s">
+        <v>10</v>
+      </c>
+      <c r="H10" t="s">
+        <v>225</v>
+      </c>
+      <c r="I10" s="4" t="s">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="11" spans="2:10" x14ac:dyDescent="0.25">
+      <c r="B11" s="6" t="s">
         <v>7</v>
       </c>
       <c r="C11" t="s">
@@ -1141,12 +1485,21 @@
       <c r="D11" t="s">
         <v>138</v>
       </c>
-      <c r="E11" t="s">
+      <c r="E11" s="4" t="s">
         <v>74</v>
       </c>
-    </row>
-    <row r="12" spans="2:5" x14ac:dyDescent="0.3">
-      <c r="B12" t="s">
+      <c r="G11" t="s">
+        <v>11</v>
+      </c>
+      <c r="H11" t="s">
+        <v>226</v>
+      </c>
+      <c r="I11" s="4" t="s">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="12" spans="2:10" x14ac:dyDescent="0.25">
+      <c r="B12" s="6" t="s">
         <v>7</v>
       </c>
       <c r="C12" t="s">
@@ -1155,12 +1508,21 @@
       <c r="D12" t="s">
         <v>139</v>
       </c>
-      <c r="E12" t="s">
+      <c r="E12" s="4" t="s">
         <v>75</v>
       </c>
-    </row>
-    <row r="13" spans="2:5" x14ac:dyDescent="0.3">
-      <c r="B13" t="s">
+      <c r="G12" t="s">
+        <v>12</v>
+      </c>
+      <c r="H12" t="s">
+        <v>227</v>
+      </c>
+      <c r="I12" s="4" t="s">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="13" spans="2:10" x14ac:dyDescent="0.25">
+      <c r="B13" s="6" t="s">
         <v>13</v>
       </c>
       <c r="C13" t="s">
@@ -1169,11 +1531,17 @@
       <c r="D13" t="s">
         <v>140</v>
       </c>
-      <c r="E13" t="s">
+      <c r="E13" s="4" t="s">
         <v>76</v>
       </c>
-    </row>
-    <row r="14" spans="2:5" x14ac:dyDescent="0.3">
+      <c r="H13" t="s">
+        <v>228</v>
+      </c>
+      <c r="I13" s="4" t="s">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="14" spans="2:10" x14ac:dyDescent="0.25">
       <c r="B14" t="s">
         <v>13</v>
       </c>
@@ -1183,12 +1551,12 @@
       <c r="D14" t="s">
         <v>141</v>
       </c>
-      <c r="E14" t="s">
+      <c r="E14" s="4" t="s">
         <v>77</v>
       </c>
     </row>
-    <row r="15" spans="2:5" x14ac:dyDescent="0.3">
-      <c r="B15" t="s">
+    <row r="15" spans="2:10" x14ac:dyDescent="0.25">
+      <c r="B15" s="6" t="s">
         <v>129</v>
       </c>
       <c r="C15" t="s">
@@ -1197,12 +1565,21 @@
       <c r="D15" t="s">
         <v>142</v>
       </c>
-      <c r="E15" t="s">
+      <c r="E15" s="4" t="s">
         <v>78</v>
       </c>
-    </row>
-    <row r="16" spans="2:5" x14ac:dyDescent="0.3">
-      <c r="B16" t="s">
+      <c r="G15" t="s">
+        <v>70</v>
+      </c>
+      <c r="H15" t="s">
+        <v>229</v>
+      </c>
+      <c r="I15" s="4" t="s">
+        <v>78</v>
+      </c>
+    </row>
+    <row r="16" spans="2:10" x14ac:dyDescent="0.25">
+      <c r="B16" s="6" t="s">
         <v>129</v>
       </c>
       <c r="C16" t="s">
@@ -1211,12 +1588,21 @@
       <c r="D16" t="s">
         <v>143</v>
       </c>
-      <c r="E16" t="s">
+      <c r="E16" s="4" t="s">
         <v>15</v>
       </c>
-    </row>
-    <row r="17" spans="2:5" x14ac:dyDescent="0.3">
-      <c r="B17" t="s">
+      <c r="G16" t="s">
+        <v>208</v>
+      </c>
+      <c r="H16" t="s">
+        <v>230</v>
+      </c>
+      <c r="I16" s="4" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="17" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="B17" s="6" t="s">
         <v>129</v>
       </c>
       <c r="C17" t="s">
@@ -1225,12 +1611,21 @@
       <c r="D17" t="s">
         <v>144</v>
       </c>
-      <c r="E17" t="s">
+      <c r="E17" s="4" t="s">
         <v>79</v>
       </c>
-    </row>
-    <row r="18" spans="2:5" x14ac:dyDescent="0.3">
-      <c r="B18" t="s">
+      <c r="G17" t="s">
+        <v>16</v>
+      </c>
+      <c r="H17" t="s">
+        <v>231</v>
+      </c>
+      <c r="I17" s="4" t="s">
+        <v>79</v>
+      </c>
+    </row>
+    <row r="18" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="B18" s="6" t="s">
         <v>17</v>
       </c>
       <c r="C18" t="s">
@@ -1239,12 +1634,21 @@
       <c r="D18" t="s">
         <v>145</v>
       </c>
-      <c r="E18" t="s">
+      <c r="E18" s="4" t="s">
         <v>80</v>
       </c>
-    </row>
-    <row r="19" spans="2:5" x14ac:dyDescent="0.3">
-      <c r="B19" t="s">
+      <c r="G18" t="s">
+        <v>209</v>
+      </c>
+      <c r="H18" t="s">
+        <v>232</v>
+      </c>
+      <c r="I18" s="4" t="s">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="19" spans="2:9" ht="30" x14ac:dyDescent="0.25">
+      <c r="B19" s="6" t="s">
         <v>17</v>
       </c>
       <c r="C19" t="s">
@@ -1253,11 +1657,20 @@
       <c r="D19" t="s">
         <v>146</v>
       </c>
-      <c r="E19" t="s">
+      <c r="E19" s="4" t="s">
         <v>115</v>
       </c>
-    </row>
-    <row r="20" spans="2:5" x14ac:dyDescent="0.3">
+      <c r="G19" t="s">
+        <v>66</v>
+      </c>
+      <c r="H19" t="s">
+        <v>233</v>
+      </c>
+      <c r="I19" s="4" t="s">
+        <v>115</v>
+      </c>
+    </row>
+    <row r="20" spans="2:9" ht="30" x14ac:dyDescent="0.25">
       <c r="B20" t="s">
         <v>19</v>
       </c>
@@ -1267,11 +1680,11 @@
       <c r="D20" t="s">
         <v>147</v>
       </c>
-      <c r="E20" t="s">
+      <c r="E20" s="4" t="s">
         <v>81</v>
       </c>
     </row>
-    <row r="21" spans="2:5" x14ac:dyDescent="0.3">
+    <row r="21" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B21" t="s">
         <v>19</v>
       </c>
@@ -1281,12 +1694,12 @@
       <c r="D21" t="s">
         <v>148</v>
       </c>
-      <c r="E21" t="s">
+      <c r="E21" s="4" t="s">
         <v>82</v>
       </c>
     </row>
-    <row r="22" spans="2:5" x14ac:dyDescent="0.3">
-      <c r="B22" t="s">
+    <row r="22" spans="2:9" ht="30" x14ac:dyDescent="0.25">
+      <c r="B22" s="6" t="s">
         <v>19</v>
       </c>
       <c r="C22" t="s">
@@ -1295,12 +1708,21 @@
       <c r="D22" t="s">
         <v>149</v>
       </c>
-      <c r="E22" t="s">
+      <c r="E22" s="4" t="s">
         <v>83</v>
       </c>
-    </row>
-    <row r="23" spans="2:5" x14ac:dyDescent="0.3">
-      <c r="B23" t="s">
+      <c r="G22" t="s">
+        <v>190</v>
+      </c>
+      <c r="H22" t="s">
+        <v>234</v>
+      </c>
+      <c r="I22" s="4" t="s">
+        <v>83</v>
+      </c>
+    </row>
+    <row r="23" spans="2:9" ht="30" x14ac:dyDescent="0.25">
+      <c r="B23" s="6" t="s">
         <v>19</v>
       </c>
       <c r="C23" t="s">
@@ -1309,12 +1731,21 @@
       <c r="D23" t="s">
         <v>150</v>
       </c>
-      <c r="E23" t="s">
+      <c r="E23" s="4" t="s">
         <v>84</v>
       </c>
-    </row>
-    <row r="24" spans="2:5" x14ac:dyDescent="0.3">
-      <c r="B24" t="s">
+      <c r="G23" t="s">
+        <v>191</v>
+      </c>
+      <c r="H23" t="s">
+        <v>235</v>
+      </c>
+      <c r="I23" s="4" t="s">
+        <v>84</v>
+      </c>
+    </row>
+    <row r="24" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="B24" s="6" t="s">
         <v>19</v>
       </c>
       <c r="C24" t="s">
@@ -1323,12 +1754,21 @@
       <c r="D24" t="s">
         <v>151</v>
       </c>
-      <c r="E24" t="s">
+      <c r="E24" s="4" t="s">
         <v>85</v>
       </c>
-    </row>
-    <row r="25" spans="2:5" x14ac:dyDescent="0.3">
-      <c r="B25" t="s">
+      <c r="G24" t="s">
+        <v>192</v>
+      </c>
+      <c r="H24" t="s">
+        <v>236</v>
+      </c>
+      <c r="I24" s="4" t="s">
+        <v>85</v>
+      </c>
+    </row>
+    <row r="25" spans="2:9" ht="30" x14ac:dyDescent="0.25">
+      <c r="B25" s="6" t="s">
         <v>19</v>
       </c>
       <c r="C25" t="s">
@@ -1337,11 +1777,20 @@
       <c r="D25" t="s">
         <v>152</v>
       </c>
-      <c r="E25" t="s">
+      <c r="E25" s="4" t="s">
         <v>86</v>
       </c>
-    </row>
-    <row r="26" spans="2:5" x14ac:dyDescent="0.3">
+      <c r="G25" t="s">
+        <v>193</v>
+      </c>
+      <c r="H25" t="s">
+        <v>237</v>
+      </c>
+      <c r="I25" s="4" t="s">
+        <v>86</v>
+      </c>
+    </row>
+    <row r="26" spans="2:9" ht="30" x14ac:dyDescent="0.25">
       <c r="B26" t="s">
         <v>19</v>
       </c>
@@ -1351,11 +1800,11 @@
       <c r="D26" t="s">
         <v>153</v>
       </c>
-      <c r="E26" t="s">
+      <c r="E26" s="4" t="s">
         <v>101</v>
       </c>
     </row>
-    <row r="27" spans="2:5" x14ac:dyDescent="0.3">
+    <row r="27" spans="2:9" ht="30" x14ac:dyDescent="0.25">
       <c r="B27" t="s">
         <v>19</v>
       </c>
@@ -1365,11 +1814,11 @@
       <c r="D27" t="s">
         <v>154</v>
       </c>
-      <c r="E27" t="s">
+      <c r="E27" s="4" t="s">
         <v>102</v>
       </c>
     </row>
-    <row r="28" spans="2:5" x14ac:dyDescent="0.3">
+    <row r="28" spans="2:9" ht="45" x14ac:dyDescent="0.25">
       <c r="B28" t="s">
         <v>19</v>
       </c>
@@ -1379,11 +1828,11 @@
       <c r="D28" t="s">
         <v>155</v>
       </c>
-      <c r="E28" t="s">
+      <c r="E28" s="4" t="s">
         <v>103</v>
       </c>
     </row>
-    <row r="29" spans="2:5" x14ac:dyDescent="0.3">
+    <row r="29" spans="2:9" ht="45" x14ac:dyDescent="0.25">
       <c r="B29" t="s">
         <v>19</v>
       </c>
@@ -1393,12 +1842,12 @@
       <c r="D29" t="s">
         <v>156</v>
       </c>
-      <c r="E29" t="s">
+      <c r="E29" s="4" t="s">
         <v>104</v>
       </c>
     </row>
-    <row r="30" spans="2:5" x14ac:dyDescent="0.3">
-      <c r="B30" t="s">
+    <row r="30" spans="2:9" ht="60" x14ac:dyDescent="0.25">
+      <c r="B30" s="6" t="s">
         <v>20</v>
       </c>
       <c r="C30" t="s">
@@ -1407,12 +1856,21 @@
       <c r="D30" t="s">
         <v>157</v>
       </c>
-      <c r="E30" t="s">
+      <c r="E30" s="4" t="s">
         <v>87</v>
       </c>
-    </row>
-    <row r="31" spans="2:5" x14ac:dyDescent="0.3">
-      <c r="B31" t="s">
+      <c r="G30" t="s">
+        <v>194</v>
+      </c>
+      <c r="H30" t="s">
+        <v>238</v>
+      </c>
+      <c r="I30" s="4" t="s">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="31" spans="2:9" ht="30" x14ac:dyDescent="0.25">
+      <c r="B31" s="6" t="s">
         <v>20</v>
       </c>
       <c r="C31" t="s">
@@ -1421,12 +1879,21 @@
       <c r="D31" t="s">
         <v>158</v>
       </c>
-      <c r="E31" t="s">
+      <c r="E31" s="4" t="s">
         <v>88</v>
       </c>
-    </row>
-    <row r="32" spans="2:5" x14ac:dyDescent="0.3">
-      <c r="B32" t="s">
+      <c r="G31" t="s">
+        <v>195</v>
+      </c>
+      <c r="H31" t="s">
+        <v>239</v>
+      </c>
+      <c r="I31" s="4" t="s">
+        <v>88</v>
+      </c>
+    </row>
+    <row r="32" spans="2:9" ht="45" x14ac:dyDescent="0.25">
+      <c r="B32" s="6" t="s">
         <v>20</v>
       </c>
       <c r="C32" t="s">
@@ -1435,12 +1902,12 @@
       <c r="D32" t="s">
         <v>159</v>
       </c>
-      <c r="E32" t="s">
+      <c r="E32" s="4" t="s">
         <v>89</v>
       </c>
     </row>
-    <row r="33" spans="2:5" x14ac:dyDescent="0.3">
-      <c r="B33" t="s">
+    <row r="33" spans="2:18" ht="30" x14ac:dyDescent="0.25">
+      <c r="B33" s="6" t="s">
         <v>20</v>
       </c>
       <c r="C33" t="s">
@@ -1449,12 +1916,27 @@
       <c r="D33" t="s">
         <v>160</v>
       </c>
-      <c r="E33" t="s">
+      <c r="E33" s="4" t="s">
         <v>90</v>
       </c>
-    </row>
-    <row r="34" spans="2:5" x14ac:dyDescent="0.3">
-      <c r="B34" t="s">
+      <c r="G33" t="s">
+        <v>197</v>
+      </c>
+      <c r="H33" t="s">
+        <v>240</v>
+      </c>
+      <c r="I33" s="4" t="s">
+        <v>90</v>
+      </c>
+      <c r="Q33" t="s">
+        <v>207</v>
+      </c>
+      <c r="R33" t="s">
+        <v>216</v>
+      </c>
+    </row>
+    <row r="34" spans="2:18" ht="30" x14ac:dyDescent="0.25">
+      <c r="B34" s="6" t="s">
         <v>20</v>
       </c>
       <c r="C34" t="s">
@@ -1463,12 +1945,21 @@
       <c r="D34" t="s">
         <v>161</v>
       </c>
-      <c r="E34" t="s">
+      <c r="E34" s="4" t="s">
         <v>91</v>
       </c>
-    </row>
-    <row r="35" spans="2:5" ht="15" x14ac:dyDescent="0.25">
-      <c r="B35" t="s">
+      <c r="G34" t="s">
+        <v>199</v>
+      </c>
+      <c r="H34" t="s">
+        <v>241</v>
+      </c>
+      <c r="I34" s="4" t="s">
+        <v>91</v>
+      </c>
+    </row>
+    <row r="35" spans="2:18" x14ac:dyDescent="0.25">
+      <c r="B35" s="6" t="s">
         <v>20</v>
       </c>
       <c r="C35" t="s">
@@ -1477,12 +1968,21 @@
       <c r="D35" t="s">
         <v>162</v>
       </c>
-      <c r="E35" t="s">
+      <c r="E35" s="4" t="s">
         <v>92</v>
       </c>
-    </row>
-    <row r="36" spans="2:5" ht="15" x14ac:dyDescent="0.25">
-      <c r="B36" t="s">
+      <c r="G35" t="s">
+        <v>198</v>
+      </c>
+      <c r="H35" t="s">
+        <v>242</v>
+      </c>
+      <c r="I35" s="4" t="s">
+        <v>92</v>
+      </c>
+    </row>
+    <row r="36" spans="2:18" ht="30" x14ac:dyDescent="0.25">
+      <c r="B36" s="6" t="s">
         <v>20</v>
       </c>
       <c r="C36" t="s">
@@ -1491,12 +1991,12 @@
       <c r="D36" t="s">
         <v>163</v>
       </c>
-      <c r="E36" t="s">
+      <c r="E36" s="4" t="s">
         <v>93</v>
       </c>
     </row>
-    <row r="37" spans="2:5" x14ac:dyDescent="0.3">
-      <c r="B37" t="s">
+    <row r="37" spans="2:18" x14ac:dyDescent="0.25">
+      <c r="B37" s="6" t="s">
         <v>20</v>
       </c>
       <c r="C37" t="s">
@@ -1505,326 +2005,529 @@
       <c r="D37" t="s">
         <v>164</v>
       </c>
-      <c r="E37" t="s">
+      <c r="E37" s="4" t="s">
         <v>94</v>
       </c>
     </row>
-    <row r="38" spans="2:5" x14ac:dyDescent="0.3">
-      <c r="B38" t="s">
+    <row r="38" spans="2:18" x14ac:dyDescent="0.25">
+      <c r="G38" t="s">
+        <v>196</v>
+      </c>
+      <c r="I38" s="4" t="s">
+        <v>214</v>
+      </c>
+    </row>
+    <row r="40" spans="2:18" ht="30" x14ac:dyDescent="0.25">
+      <c r="B40" s="6" t="s">
         <v>21</v>
       </c>
-      <c r="C38" t="s">
+      <c r="C40" t="s">
         <v>55</v>
       </c>
-      <c r="D38" t="s">
+      <c r="D40" t="s">
         <v>165</v>
       </c>
-      <c r="E38" t="s">
+      <c r="E40" s="4" t="s">
         <v>95</v>
       </c>
-    </row>
-    <row r="39" spans="2:5" ht="15" x14ac:dyDescent="0.25">
-      <c r="B39" t="s">
+      <c r="G40" t="s">
+        <v>200</v>
+      </c>
+      <c r="H40" t="s">
+        <v>243</v>
+      </c>
+      <c r="I40" s="4" t="s">
+        <v>95</v>
+      </c>
+    </row>
+    <row r="41" spans="2:18" ht="30" x14ac:dyDescent="0.25">
+      <c r="B41" s="6" t="s">
         <v>21</v>
       </c>
-      <c r="C39" t="s">
+      <c r="C41" t="s">
         <v>56</v>
       </c>
-      <c r="D39" t="s">
+      <c r="D41" t="s">
         <v>166</v>
       </c>
-      <c r="E39" t="s">
+      <c r="E41" s="4" t="s">
         <v>96</v>
       </c>
-    </row>
-    <row r="40" spans="2:5" x14ac:dyDescent="0.3">
-      <c r="B40" t="s">
+      <c r="G41" t="s">
+        <v>201</v>
+      </c>
+      <c r="H41" t="s">
+        <v>244</v>
+      </c>
+      <c r="I41" s="4" t="s">
+        <v>96</v>
+      </c>
+    </row>
+    <row r="42" spans="2:18" ht="30" x14ac:dyDescent="0.25">
+      <c r="B42" s="6" t="s">
         <v>21</v>
       </c>
-      <c r="C40" t="s">
+      <c r="C42" t="s">
         <v>57</v>
       </c>
-      <c r="D40" t="s">
+      <c r="D42" t="s">
         <v>167</v>
       </c>
-      <c r="E40" t="s">
+      <c r="E42" s="4" t="s">
         <v>97</v>
       </c>
-    </row>
-    <row r="41" spans="2:5" x14ac:dyDescent="0.3">
-      <c r="B41" t="s">
+      <c r="G42" t="s">
+        <v>202</v>
+      </c>
+      <c r="H42" t="s">
+        <v>245</v>
+      </c>
+      <c r="I42" s="4" t="s">
+        <v>97</v>
+      </c>
+    </row>
+    <row r="43" spans="2:18" ht="30" x14ac:dyDescent="0.25">
+      <c r="B43" s="6" t="s">
         <v>21</v>
       </c>
-      <c r="C41" t="s">
+      <c r="C43" t="s">
         <v>58</v>
       </c>
-      <c r="D41" t="s">
+      <c r="D43" t="s">
         <v>168</v>
       </c>
-      <c r="E41" t="s">
+      <c r="E43" s="4" t="s">
         <v>98</v>
       </c>
-    </row>
-    <row r="42" spans="2:5" x14ac:dyDescent="0.3">
-      <c r="B42" t="s">
+      <c r="G43" t="s">
+        <v>203</v>
+      </c>
+      <c r="H43" t="s">
+        <v>246</v>
+      </c>
+      <c r="I43" s="4" t="s">
+        <v>98</v>
+      </c>
+    </row>
+    <row r="44" spans="2:18" ht="30" x14ac:dyDescent="0.25">
+      <c r="B44" s="6" t="s">
         <v>21</v>
       </c>
-      <c r="C42" t="s">
+      <c r="C44" t="s">
         <v>59</v>
       </c>
-      <c r="D42" t="s">
+      <c r="D44" t="s">
         <v>169</v>
       </c>
-      <c r="E42" t="s">
+      <c r="E44" s="4" t="s">
         <v>99</v>
       </c>
-    </row>
-    <row r="43" spans="2:5" x14ac:dyDescent="0.3">
-      <c r="B43" t="s">
+      <c r="G44" t="s">
+        <v>204</v>
+      </c>
+      <c r="H44" t="s">
+        <v>247</v>
+      </c>
+      <c r="I44" s="4" t="s">
+        <v>99</v>
+      </c>
+    </row>
+    <row r="45" spans="2:18" x14ac:dyDescent="0.25">
+      <c r="B45" s="6" t="s">
         <v>21</v>
       </c>
-      <c r="C43" t="s">
+      <c r="C45" t="s">
         <v>60</v>
       </c>
-      <c r="D43" t="s">
+      <c r="D45" t="s">
         <v>170</v>
       </c>
-      <c r="E43" t="s">
+      <c r="E45" s="4" t="s">
         <v>100</v>
       </c>
-    </row>
-    <row r="44" spans="2:5" x14ac:dyDescent="0.3">
-      <c r="B44" t="s">
+      <c r="G45" t="s">
+        <v>205</v>
+      </c>
+      <c r="H45" t="s">
+        <v>248</v>
+      </c>
+      <c r="I45" s="4" t="s">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="46" spans="2:18" ht="30" x14ac:dyDescent="0.25">
+      <c r="B46" s="6" t="s">
         <v>22</v>
       </c>
-      <c r="C44" t="s">
+      <c r="C46" t="s">
         <v>61</v>
       </c>
-      <c r="D44" t="s">
+      <c r="D46" t="s">
         <v>171</v>
       </c>
-      <c r="E44" t="s">
-        <v>22</v>
-      </c>
-    </row>
-    <row r="45" spans="2:5" x14ac:dyDescent="0.3">
-      <c r="B45" t="s">
+      <c r="E46" s="4" t="s">
+        <v>215</v>
+      </c>
+      <c r="G46" t="s">
+        <v>206</v>
+      </c>
+      <c r="H46" t="s">
+        <v>249</v>
+      </c>
+      <c r="I46" s="4" t="s">
+        <v>215</v>
+      </c>
+    </row>
+    <row r="47" spans="2:18" x14ac:dyDescent="0.25">
+      <c r="B47" s="6" t="s">
         <v>23</v>
       </c>
-      <c r="C45" t="s">
+      <c r="C47" t="s">
         <v>24</v>
       </c>
-      <c r="D45" t="s">
+      <c r="D47" t="s">
         <v>172</v>
       </c>
-      <c r="E45" t="s">
+      <c r="E47" s="4" t="s">
         <v>110</v>
       </c>
-    </row>
-    <row r="46" spans="2:5" ht="15" x14ac:dyDescent="0.25">
-      <c r="B46" t="s">
+      <c r="G47" t="s">
+        <v>24</v>
+      </c>
+      <c r="H47" t="s">
+        <v>250</v>
+      </c>
+      <c r="I47" s="4" t="s">
+        <v>110</v>
+      </c>
+    </row>
+    <row r="48" spans="2:18" x14ac:dyDescent="0.25">
+      <c r="B48" s="6" t="s">
         <v>23</v>
       </c>
-      <c r="C46" t="s">
+      <c r="C48" t="s">
         <v>62</v>
       </c>
-      <c r="D46" t="s">
+      <c r="D48" t="s">
         <v>173</v>
       </c>
-      <c r="E46" t="s">
+      <c r="E48" s="4" t="s">
         <v>111</v>
       </c>
-    </row>
-    <row r="47" spans="2:5" ht="15" x14ac:dyDescent="0.25">
-      <c r="B47" t="s">
+      <c r="G48" t="s">
+        <v>62</v>
+      </c>
+      <c r="H48" t="s">
+        <v>251</v>
+      </c>
+      <c r="I48" s="4" t="s">
+        <v>111</v>
+      </c>
+    </row>
+    <row r="49" spans="2:18" ht="30" x14ac:dyDescent="0.25">
+      <c r="B49" s="6" t="s">
         <v>23</v>
       </c>
-      <c r="C47" t="s">
+      <c r="C49" t="s">
         <v>63</v>
       </c>
-      <c r="D47" t="s">
+      <c r="D49" t="s">
         <v>174</v>
       </c>
-      <c r="E47" t="s">
+      <c r="E49" s="4" t="s">
         <v>112</v>
       </c>
-    </row>
-    <row r="48" spans="2:5" x14ac:dyDescent="0.3">
-      <c r="B48" t="s">
+      <c r="G49" t="s">
+        <v>63</v>
+      </c>
+      <c r="H49" t="s">
+        <v>252</v>
+      </c>
+      <c r="I49" s="4" t="s">
+        <v>112</v>
+      </c>
+      <c r="Q49" t="s">
+        <v>210</v>
+      </c>
+      <c r="R49" t="s">
+        <v>217</v>
+      </c>
+    </row>
+    <row r="50" spans="2:18" ht="45" x14ac:dyDescent="0.25">
+      <c r="B50" s="6" t="s">
         <v>23</v>
       </c>
-      <c r="C48" t="s">
+      <c r="C50" t="s">
         <v>64</v>
       </c>
-      <c r="D48" t="s">
+      <c r="D50" t="s">
         <v>175</v>
       </c>
-      <c r="E48" t="s">
+      <c r="E50" s="4" t="s">
         <v>113</v>
       </c>
-    </row>
-    <row r="49" spans="2:5" x14ac:dyDescent="0.3">
-      <c r="B49" t="s">
+      <c r="G50" t="s">
+        <v>64</v>
+      </c>
+      <c r="H50" t="s">
+        <v>253</v>
+      </c>
+      <c r="I50" s="4" t="s">
+        <v>113</v>
+      </c>
+      <c r="Q50" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="51" spans="2:18" x14ac:dyDescent="0.25">
+      <c r="B51" s="6" t="s">
         <v>23</v>
       </c>
-      <c r="C49" t="s">
+      <c r="C51" t="s">
         <v>65</v>
       </c>
-      <c r="D49" t="s">
+      <c r="D51" t="s">
         <v>176</v>
       </c>
-      <c r="E49" t="s">
+      <c r="E51" s="4" t="s">
         <v>114</v>
       </c>
-    </row>
-    <row r="50" spans="2:5" x14ac:dyDescent="0.3">
-      <c r="B50" t="s">
+      <c r="G51" t="s">
+        <v>65</v>
+      </c>
+      <c r="H51" t="s">
+        <v>254</v>
+      </c>
+      <c r="I51" s="4" t="s">
+        <v>114</v>
+      </c>
+    </row>
+    <row r="52" spans="2:18" x14ac:dyDescent="0.25">
+      <c r="B52" s="6" t="s">
         <v>25</v>
       </c>
-      <c r="C50" t="s">
+      <c r="C52" t="s">
         <v>117</v>
       </c>
-      <c r="D50" t="s">
+      <c r="D52" t="s">
         <v>177</v>
       </c>
-      <c r="E50" t="s">
+      <c r="E52" s="4" t="s">
         <v>116</v>
       </c>
-    </row>
-    <row r="51" spans="2:5" x14ac:dyDescent="0.3">
-      <c r="B51" t="s">
+      <c r="G52" t="s">
+        <v>117</v>
+      </c>
+      <c r="H52" t="s">
+        <v>255</v>
+      </c>
+      <c r="I52" s="4" t="s">
+        <v>116</v>
+      </c>
+    </row>
+    <row r="53" spans="2:18" x14ac:dyDescent="0.25">
+      <c r="B53" s="6" t="s">
         <v>25</v>
       </c>
-      <c r="C51" t="s">
+      <c r="C53" t="s">
         <v>118</v>
       </c>
-      <c r="D51" t="s">
+      <c r="D53" t="s">
         <v>178</v>
       </c>
-      <c r="E51" t="s">
+      <c r="E53" s="4" t="s">
         <v>121</v>
       </c>
-    </row>
-    <row r="52" spans="2:5" ht="15" x14ac:dyDescent="0.25">
-      <c r="B52" t="s">
+      <c r="G53" t="s">
+        <v>118</v>
+      </c>
+      <c r="H53" t="s">
+        <v>256</v>
+      </c>
+      <c r="I53" s="4" t="s">
+        <v>121</v>
+      </c>
+    </row>
+    <row r="54" spans="2:18" x14ac:dyDescent="0.25">
+      <c r="B54" s="6" t="s">
         <v>25</v>
       </c>
-      <c r="C52" t="s">
+      <c r="C54" t="s">
         <v>119</v>
       </c>
-      <c r="D52" t="s">
+      <c r="D54" t="s">
         <v>179</v>
       </c>
-      <c r="E52" t="s">
+      <c r="E54" s="4" t="s">
         <v>122</v>
       </c>
-    </row>
-    <row r="53" spans="2:5" x14ac:dyDescent="0.3">
-      <c r="B53" t="s">
+      <c r="G54" t="s">
+        <v>119</v>
+      </c>
+      <c r="H54" t="s">
+        <v>257</v>
+      </c>
+      <c r="I54" s="4" t="s">
+        <v>122</v>
+      </c>
+    </row>
+    <row r="55" spans="2:18" x14ac:dyDescent="0.25">
+      <c r="B55" s="6" t="s">
         <v>25</v>
       </c>
-      <c r="C53" t="s">
+      <c r="C55" t="s">
         <v>120</v>
       </c>
-      <c r="D53" t="s">
+      <c r="D55" t="s">
         <v>180</v>
       </c>
-      <c r="E53" t="s">
+      <c r="E55" s="4" t="s">
         <v>123</v>
       </c>
-    </row>
-    <row r="54" spans="2:5" x14ac:dyDescent="0.3">
-      <c r="B54" t="s">
+      <c r="G55" t="s">
+        <v>120</v>
+      </c>
+      <c r="H55" t="s">
+        <v>258</v>
+      </c>
+      <c r="I55" s="4" t="s">
+        <v>123</v>
+      </c>
+    </row>
+    <row r="56" spans="2:18" x14ac:dyDescent="0.25">
+      <c r="B56" s="6" t="s">
         <v>126</v>
       </c>
-      <c r="C54" t="s">
+      <c r="C56" t="s">
         <v>68</v>
       </c>
-      <c r="D54" t="s">
+      <c r="D56" t="s">
         <v>181</v>
       </c>
-      <c r="E54" t="s">
+      <c r="E56" s="4" t="s">
         <v>124</v>
       </c>
-    </row>
-    <row r="55" spans="2:5" x14ac:dyDescent="0.3">
-      <c r="B55" t="s">
+      <c r="G56" t="s">
+        <v>211</v>
+      </c>
+      <c r="H56" t="s">
+        <v>259</v>
+      </c>
+      <c r="I56" s="4" t="s">
+        <v>124</v>
+      </c>
+    </row>
+    <row r="57" spans="2:18" x14ac:dyDescent="0.25">
+      <c r="B57" s="6" t="s">
         <v>126</v>
       </c>
-      <c r="C55" t="s">
+      <c r="C57" t="s">
         <v>67</v>
       </c>
-      <c r="D55" t="s">
+      <c r="D57" t="s">
         <v>182</v>
       </c>
-      <c r="E55" t="s">
+      <c r="E57" s="4" t="s">
         <v>125</v>
       </c>
-    </row>
-    <row r="56" spans="2:5" x14ac:dyDescent="0.3">
-      <c r="B56" t="s">
+      <c r="G57" t="s">
+        <v>67</v>
+      </c>
+      <c r="H57" t="s">
+        <v>260</v>
+      </c>
+      <c r="I57" s="4" t="s">
+        <v>125</v>
+      </c>
+    </row>
+    <row r="58" spans="2:18" x14ac:dyDescent="0.25">
+      <c r="B58" s="6" t="s">
         <v>127</v>
       </c>
-      <c r="C56" t="s">
+      <c r="C58" t="s">
         <v>26</v>
       </c>
-      <c r="D56" t="s">
+      <c r="D58" t="s">
         <v>183</v>
       </c>
-    </row>
-    <row r="57" spans="2:5" x14ac:dyDescent="0.3">
-      <c r="B57" t="s">
+      <c r="G58" t="s">
+        <v>212</v>
+      </c>
+      <c r="H58" t="s">
+        <v>261</v>
+      </c>
+    </row>
+    <row r="59" spans="2:18" x14ac:dyDescent="0.25">
+      <c r="B59" s="6" t="s">
         <v>127</v>
       </c>
-      <c r="C57" t="s">
+      <c r="C59" t="s">
         <v>27</v>
       </c>
-      <c r="D57" t="s">
+      <c r="D59" t="s">
         <v>184</v>
       </c>
-    </row>
-    <row r="58" spans="2:5" x14ac:dyDescent="0.3">
-      <c r="B58" t="s">
+      <c r="G59" t="s">
+        <v>213</v>
+      </c>
+      <c r="H59" t="s">
+        <v>262</v>
+      </c>
+    </row>
+    <row r="60" spans="2:18" x14ac:dyDescent="0.25">
+      <c r="B60" s="6" t="s">
         <v>128</v>
       </c>
-      <c r="C58" t="s">
+      <c r="C60" t="s">
         <v>28</v>
       </c>
-      <c r="D58" t="s">
+      <c r="D60" t="s">
         <v>185</v>
       </c>
-    </row>
-    <row r="59" spans="2:5" x14ac:dyDescent="0.3">
-      <c r="B59" t="s">
-        <v>128</v>
-      </c>
-      <c r="C59" t="s">
-        <v>29</v>
-      </c>
-      <c r="D59" t="s">
-        <v>186</v>
-      </c>
-    </row>
-    <row r="60" spans="2:5" x14ac:dyDescent="0.3">
-      <c r="B60" t="s">
-        <v>128</v>
-      </c>
-      <c r="C60" t="s">
-        <v>30</v>
-      </c>
-      <c r="D60" t="s">
-        <v>187</v>
-      </c>
-    </row>
-    <row r="61" spans="2:5" x14ac:dyDescent="0.3">
+      <c r="G60" t="s">
+        <v>189</v>
+      </c>
+      <c r="H60" t="s">
+        <v>263</v>
+      </c>
+    </row>
+    <row r="61" spans="2:18" x14ac:dyDescent="0.25">
       <c r="B61" t="s">
         <v>128</v>
       </c>
       <c r="C61" t="s">
+        <v>29</v>
+      </c>
+      <c r="D61" t="s">
+        <v>186</v>
+      </c>
+    </row>
+    <row r="62" spans="2:18" x14ac:dyDescent="0.25">
+      <c r="B62" t="s">
+        <v>128</v>
+      </c>
+      <c r="C62" t="s">
+        <v>30</v>
+      </c>
+      <c r="D62" t="s">
+        <v>187</v>
+      </c>
+    </row>
+    <row r="63" spans="2:18" x14ac:dyDescent="0.25">
+      <c r="B63" s="6" t="s">
+        <v>128</v>
+      </c>
+      <c r="C63" t="s">
         <v>31</v>
       </c>
-      <c r="D61" t="s">
+      <c r="D63" t="s">
         <v>188</v>
+      </c>
+      <c r="G63" t="s">
+        <v>31</v>
+      </c>
+      <c r="H63" t="s">
+        <v>264</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Adding CCES 2014 Data
Updated Sqlite with 2014 Data
Updated Variable Index with 2014 Data
</commit_message>
<xml_diff>
--- a/Variable_Index.xlsx
+++ b/Variable_Index.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Owner\OneDrive\tempschool\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="492" documentId="8_{5BB726C6-045A-4B74-832F-0E45B46FDC8E}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{F41D8518-C3E8-4AF1-BF7A-9BCA7FE6CE58}"/>
+  <xr:revisionPtr revIDLastSave="675" documentId="8_{5BB726C6-045A-4B74-832F-0E45B46FDC8E}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{2D89EAC6-C6BF-44AC-A125-F994D3D4C087}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="13800" windowHeight="4410" xr2:uid="{B1787686-8DD4-4EAF-A6DB-220586B0E0A3}"/>
   </bookViews>
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="382" uniqueCount="266">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3214" uniqueCount="328">
   <si>
     <t>ID</t>
   </si>
@@ -621,9 +621,6 @@
     <t>CC15_321_2</t>
   </si>
   <si>
-    <t>CC15_321_3</t>
-  </si>
-  <si>
     <t>CC15_321_4</t>
   </si>
   <si>
@@ -675,9 +672,6 @@
     <t>endtime</t>
   </si>
   <si>
-    <t>Allow police to question anyone they think may be in the country illegally.</t>
-  </si>
-  <si>
     <t>Do you favor or oppose allowing gays and lesbians to marry legally?</t>
   </si>
   <si>
@@ -829,6 +823,198 @@
   </si>
   <si>
     <t>CCES_2015</t>
+  </si>
+  <si>
+    <t>CCES_2014</t>
+  </si>
+  <si>
+    <t>CC14_320a</t>
+  </si>
+  <si>
+    <t>CC14_320b</t>
+  </si>
+  <si>
+    <t>CC14_320d</t>
+  </si>
+  <si>
+    <t>CC14_320e</t>
+  </si>
+  <si>
+    <t>CC14_322_1</t>
+  </si>
+  <si>
+    <t>CC14_322_2</t>
+  </si>
+  <si>
+    <t>CC14_322_4</t>
+  </si>
+  <si>
+    <t>CC14_322_5</t>
+  </si>
+  <si>
+    <t>CC14_322_6</t>
+  </si>
+  <si>
+    <t>CC14_323_1</t>
+  </si>
+  <si>
+    <t>CC14_323_2</t>
+  </si>
+  <si>
+    <t>CC14_323_3</t>
+  </si>
+  <si>
+    <t>CC14_323_4</t>
+  </si>
+  <si>
+    <t>CC14_323_5</t>
+  </si>
+  <si>
+    <t>CC14_327</t>
+  </si>
+  <si>
+    <t>V101_14</t>
+  </si>
+  <si>
+    <t>Zipcode_14</t>
+  </si>
+  <si>
+    <t>State_14</t>
+  </si>
+  <si>
+    <t>CountyFips_14</t>
+  </si>
+  <si>
+    <t>CountyName_14</t>
+  </si>
+  <si>
+    <t>Birth Year_14</t>
+  </si>
+  <si>
+    <t>Gender_14</t>
+  </si>
+  <si>
+    <t>Education_14</t>
+  </si>
+  <si>
+    <t>Race_14</t>
+  </si>
+  <si>
+    <t>Marrital Status_14</t>
+  </si>
+  <si>
+    <t>Children &lt; 18 yrs_14</t>
+  </si>
+  <si>
+    <t>Immigration Status_14</t>
+  </si>
+  <si>
+    <t>Family Income_14</t>
+  </si>
+  <si>
+    <t>Employment Status_14</t>
+  </si>
+  <si>
+    <t>Own Home_14</t>
+  </si>
+  <si>
+    <t>Political Preference_14</t>
+  </si>
+  <si>
+    <t>Political Viewpoint_14</t>
+  </si>
+  <si>
+    <t>Gun Background Checks_14</t>
+  </si>
+  <si>
+    <t>Prohibit Publication_14</t>
+  </si>
+  <si>
+    <t>Ban Assult Weapons_14</t>
+  </si>
+  <si>
+    <t>Make CCP Easier_14</t>
+  </si>
+  <si>
+    <t>Grant Legal Status_14</t>
+  </si>
+  <si>
+    <t>Increase Border Patrols_14</t>
+  </si>
+  <si>
+    <t>Fine employers_14</t>
+  </si>
+  <si>
+    <t>Identify and deport_14</t>
+  </si>
+  <si>
+    <t>No to all_14</t>
+  </si>
+  <si>
+    <t>Always Allow Choice_14</t>
+  </si>
+  <si>
+    <t>Rape, Incest, or Health_14</t>
+  </si>
+  <si>
+    <t>Prohibit &gt; 20 Weeks_14</t>
+  </si>
+  <si>
+    <t>Employers decline benefits_14</t>
+  </si>
+  <si>
+    <t>Prohibit Fed Funds_14</t>
+  </si>
+  <si>
+    <t>Gay Marriage_14</t>
+  </si>
+  <si>
+    <t>Bornagain_14</t>
+  </si>
+  <si>
+    <t>Religious Importance_14</t>
+  </si>
+  <si>
+    <t>Church Attendance_14</t>
+  </si>
+  <si>
+    <t>Prayer Frequency_14</t>
+  </si>
+  <si>
+    <t>Religion Donomination_14</t>
+  </si>
+  <si>
+    <t>Military - I am_14</t>
+  </si>
+  <si>
+    <t>Military - Family_14</t>
+  </si>
+  <si>
+    <t>Military - I served_14</t>
+  </si>
+  <si>
+    <t>Military - Family served_14</t>
+  </si>
+  <si>
+    <t>Union - Self_14</t>
+  </si>
+  <si>
+    <t>Union - Family_14</t>
+  </si>
+  <si>
+    <t>starttime_pre_14</t>
+  </si>
+  <si>
+    <t>endtime_pre_14</t>
+  </si>
+  <si>
+    <t>commonweight_14</t>
+  </si>
+  <si>
+    <t>ccesmodule_14</t>
+  </si>
+  <si>
+    <t>YES</t>
   </si>
 </sst>
 </file>
@@ -867,7 +1053,7 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.39997558519241921"/>
+        <fgColor rgb="FF92D050"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -884,7 +1070,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="7">
+  <cellXfs count="9">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
@@ -895,6 +1081,8 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
@@ -1238,48 +1426,59 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8B0C4685-FCD9-4520-9F28-50A98CF8260A}">
-  <dimension ref="B1:R63"/>
+  <dimension ref="A1:V61"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="J1" sqref="J1:J1048576"/>
+    <sheetView tabSelected="1" topLeftCell="A48" workbookViewId="0">
+      <selection activeCell="A61" sqref="A61"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="2" max="2" width="12.5703125" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="24.5703125" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="42.5703125" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="49.5703125" style="4" customWidth="1"/>
-    <col min="6" max="6" width="2" style="2" customWidth="1"/>
-    <col min="7" max="7" width="14.85546875" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="28.7109375" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="39.140625" style="4" customWidth="1"/>
+    <col min="1" max="1" width="12.5703125" style="6" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="2" style="2" customWidth="1"/>
+    <col min="6" max="6" width="12.5703125" style="6" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="24.5703125" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="37.42578125" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="33.42578125" style="4" customWidth="1"/>
     <col min="10" max="10" width="2" style="2" customWidth="1"/>
-    <col min="12" max="12" width="14.85546875" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="14.85546875" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="28.7109375" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="31.7109375" style="4" customWidth="1"/>
+    <col min="14" max="14" width="2" style="2" customWidth="1"/>
+    <col min="15" max="15" width="14.85546875" bestFit="1" customWidth="1"/>
+    <col min="16" max="16" width="25.28515625" bestFit="1" customWidth="1"/>
+    <col min="17" max="17" width="33.7109375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="2:10" x14ac:dyDescent="0.25">
-      <c r="C1" t="s">
+    <row r="1" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="G1" t="s">
         <v>32</v>
       </c>
-      <c r="G1" t="s">
-        <v>265</v>
-      </c>
-    </row>
-    <row r="2" spans="2:10" s="1" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="B2" s="1" t="s">
+      <c r="K1" t="s">
+        <v>263</v>
+      </c>
+      <c r="O1" t="s">
+        <v>264</v>
+      </c>
+      <c r="Q1" s="4"/>
+    </row>
+    <row r="2" spans="1:17" s="1" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A2" s="7" t="s">
         <v>34</v>
       </c>
-      <c r="C2" s="1" t="s">
-        <v>35</v>
-      </c>
-      <c r="D2" s="1" t="s">
-        <v>36</v>
-      </c>
-      <c r="E2" s="5" t="s">
-        <v>33</v>
-      </c>
-      <c r="F2" s="3"/>
+      <c r="B2" s="1">
+        <v>2016</v>
+      </c>
+      <c r="C2" s="1">
+        <v>2015</v>
+      </c>
+      <c r="D2" s="1">
+        <v>2014</v>
+      </c>
+      <c r="E2" s="3"/>
+      <c r="F2" s="7" t="s">
+        <v>34</v>
+      </c>
       <c r="G2" s="1" t="s">
         <v>35</v>
       </c>
@@ -1290,1244 +1489,2302 @@
         <v>33</v>
       </c>
       <c r="J2" s="3"/>
-    </row>
-    <row r="3" spans="2:10" x14ac:dyDescent="0.25">
-      <c r="B3" s="6" t="s">
+      <c r="K2" s="1" t="s">
+        <v>35</v>
+      </c>
+      <c r="L2" s="1" t="s">
+        <v>36</v>
+      </c>
+      <c r="M2" s="5" t="s">
+        <v>33</v>
+      </c>
+      <c r="N2" s="3"/>
+      <c r="O2" s="1" t="s">
+        <v>35</v>
+      </c>
+      <c r="P2" s="1" t="s">
+        <v>36</v>
+      </c>
+      <c r="Q2" s="5" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="3" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A3" s="8" t="s">
         <v>0</v>
       </c>
+      <c r="B3" t="s">
+        <v>327</v>
+      </c>
       <c r="C3" t="s">
-        <v>1</v>
+        <v>327</v>
       </c>
       <c r="D3" t="s">
-        <v>130</v>
-      </c>
-      <c r="E3" s="4" t="s">
-        <v>105</v>
+        <v>327</v>
+      </c>
+      <c r="F3" s="6" t="s">
+        <v>0</v>
       </c>
       <c r="G3" t="s">
         <v>1</v>
       </c>
       <c r="H3" t="s">
-        <v>218</v>
+        <v>130</v>
       </c>
       <c r="I3" s="4" t="s">
         <v>105</v>
       </c>
-    </row>
-    <row r="4" spans="2:10" x14ac:dyDescent="0.25">
-      <c r="B4" s="6" t="s">
+      <c r="K3" t="s">
+        <v>1</v>
+      </c>
+      <c r="L3" t="s">
+        <v>216</v>
+      </c>
+      <c r="M3" s="4" t="s">
+        <v>105</v>
+      </c>
+      <c r="O3" t="s">
+        <v>1</v>
+      </c>
+      <c r="P3" t="s">
+        <v>280</v>
+      </c>
+      <c r="Q3" s="4" t="s">
+        <v>105</v>
+      </c>
+    </row>
+    <row r="4" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A4" s="8" t="s">
         <v>2</v>
       </c>
+      <c r="B4" t="s">
+        <v>327</v>
+      </c>
       <c r="C4" t="s">
-        <v>3</v>
+        <v>327</v>
       </c>
       <c r="D4" t="s">
-        <v>131</v>
-      </c>
-      <c r="E4" s="4" t="s">
-        <v>106</v>
+        <v>327</v>
+      </c>
+      <c r="F4" s="6" t="s">
+        <v>2</v>
       </c>
       <c r="G4" t="s">
         <v>3</v>
       </c>
       <c r="H4" t="s">
-        <v>219</v>
+        <v>131</v>
       </c>
       <c r="I4" s="4" t="s">
         <v>106</v>
       </c>
-    </row>
-    <row r="5" spans="2:10" x14ac:dyDescent="0.25">
-      <c r="B5" s="6" t="s">
+      <c r="K4" t="s">
+        <v>3</v>
+      </c>
+      <c r="L4" t="s">
+        <v>217</v>
+      </c>
+      <c r="M4" s="4" t="s">
+        <v>106</v>
+      </c>
+      <c r="O4" t="s">
+        <v>3</v>
+      </c>
+      <c r="P4" t="s">
+        <v>281</v>
+      </c>
+      <c r="Q4" s="4" t="s">
+        <v>106</v>
+      </c>
+    </row>
+    <row r="5" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A5" s="8" t="s">
         <v>2</v>
       </c>
+      <c r="B5" t="s">
+        <v>327</v>
+      </c>
       <c r="C5" t="s">
-        <v>4</v>
+        <v>327</v>
       </c>
       <c r="D5" t="s">
-        <v>132</v>
-      </c>
-      <c r="E5" s="4" t="s">
-        <v>107</v>
+        <v>327</v>
+      </c>
+      <c r="F5" s="6" t="s">
+        <v>2</v>
       </c>
       <c r="G5" t="s">
         <v>4</v>
       </c>
       <c r="H5" t="s">
-        <v>220</v>
+        <v>132</v>
       </c>
       <c r="I5" s="4" t="s">
         <v>107</v>
       </c>
-    </row>
-    <row r="6" spans="2:10" x14ac:dyDescent="0.25">
-      <c r="B6" s="6" t="s">
+      <c r="K5" t="s">
+        <v>4</v>
+      </c>
+      <c r="L5" t="s">
+        <v>218</v>
+      </c>
+      <c r="M5" s="4" t="s">
+        <v>107</v>
+      </c>
+      <c r="O5" t="s">
+        <v>4</v>
+      </c>
+      <c r="P5" t="s">
+        <v>282</v>
+      </c>
+      <c r="Q5" s="4" t="s">
+        <v>107</v>
+      </c>
+    </row>
+    <row r="6" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A6" s="8" t="s">
         <v>2</v>
       </c>
+      <c r="B6" t="s">
+        <v>327</v>
+      </c>
       <c r="C6" t="s">
-        <v>5</v>
+        <v>327</v>
       </c>
       <c r="D6" t="s">
-        <v>133</v>
-      </c>
-      <c r="E6" s="4" t="s">
-        <v>108</v>
+        <v>327</v>
+      </c>
+      <c r="F6" s="6" t="s">
+        <v>2</v>
       </c>
       <c r="G6" t="s">
         <v>5</v>
       </c>
       <c r="H6" t="s">
-        <v>221</v>
+        <v>133</v>
       </c>
       <c r="I6" s="4" t="s">
         <v>108</v>
       </c>
-    </row>
-    <row r="7" spans="2:10" x14ac:dyDescent="0.25">
-      <c r="B7" s="6" t="s">
+      <c r="K6" t="s">
+        <v>5</v>
+      </c>
+      <c r="L6" t="s">
+        <v>219</v>
+      </c>
+      <c r="M6" s="4" t="s">
+        <v>108</v>
+      </c>
+      <c r="O6" t="s">
+        <v>5</v>
+      </c>
+      <c r="P6" t="s">
+        <v>283</v>
+      </c>
+      <c r="Q6" s="4" t="s">
+        <v>108</v>
+      </c>
+    </row>
+    <row r="7" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A7" s="8" t="s">
         <v>2</v>
       </c>
+      <c r="B7" t="s">
+        <v>327</v>
+      </c>
       <c r="C7" t="s">
-        <v>6</v>
+        <v>327</v>
       </c>
       <c r="D7" t="s">
-        <v>134</v>
-      </c>
-      <c r="E7" s="4" t="s">
-        <v>109</v>
+        <v>327</v>
+      </c>
+      <c r="F7" s="6" t="s">
+        <v>2</v>
       </c>
       <c r="G7" t="s">
         <v>6</v>
       </c>
       <c r="H7" t="s">
-        <v>222</v>
+        <v>134</v>
       </c>
       <c r="I7" s="4" t="s">
         <v>109</v>
       </c>
-    </row>
-    <row r="8" spans="2:10" x14ac:dyDescent="0.25">
-      <c r="B8" s="6" t="s">
+      <c r="K7" t="s">
+        <v>6</v>
+      </c>
+      <c r="L7" t="s">
+        <v>220</v>
+      </c>
+      <c r="M7" s="4" t="s">
+        <v>109</v>
+      </c>
+      <c r="O7" t="s">
+        <v>6</v>
+      </c>
+      <c r="P7" t="s">
+        <v>284</v>
+      </c>
+      <c r="Q7" s="4" t="s">
+        <v>109</v>
+      </c>
+    </row>
+    <row r="8" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A8" s="8" t="s">
         <v>7</v>
       </c>
+      <c r="B8" t="s">
+        <v>327</v>
+      </c>
       <c r="C8" t="s">
-        <v>8</v>
+        <v>327</v>
       </c>
       <c r="D8" t="s">
-        <v>135</v>
-      </c>
-      <c r="E8" s="4" t="s">
-        <v>71</v>
+        <v>327</v>
+      </c>
+      <c r="F8" s="6" t="s">
+        <v>7</v>
       </c>
       <c r="G8" t="s">
         <v>8</v>
       </c>
       <c r="H8" t="s">
-        <v>223</v>
+        <v>135</v>
       </c>
       <c r="I8" s="4" t="s">
         <v>71</v>
       </c>
-    </row>
-    <row r="9" spans="2:10" x14ac:dyDescent="0.25">
-      <c r="B9" s="6" t="s">
+      <c r="K8" t="s">
+        <v>8</v>
+      </c>
+      <c r="L8" t="s">
+        <v>221</v>
+      </c>
+      <c r="M8" s="4" t="s">
+        <v>71</v>
+      </c>
+      <c r="O8" t="s">
+        <v>8</v>
+      </c>
+      <c r="P8" t="s">
+        <v>285</v>
+      </c>
+      <c r="Q8" s="4" t="s">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="9" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A9" s="8" t="s">
         <v>7</v>
       </c>
+      <c r="B9" t="s">
+        <v>327</v>
+      </c>
       <c r="C9" t="s">
-        <v>9</v>
+        <v>327</v>
       </c>
       <c r="D9" t="s">
-        <v>136</v>
-      </c>
-      <c r="E9" s="4" t="s">
-        <v>72</v>
+        <v>327</v>
+      </c>
+      <c r="F9" s="6" t="s">
+        <v>7</v>
       </c>
       <c r="G9" t="s">
         <v>9</v>
       </c>
       <c r="H9" t="s">
-        <v>224</v>
+        <v>136</v>
       </c>
       <c r="I9" s="4" t="s">
         <v>72</v>
       </c>
-    </row>
-    <row r="10" spans="2:10" x14ac:dyDescent="0.25">
-      <c r="B10" s="6" t="s">
+      <c r="K9" t="s">
+        <v>9</v>
+      </c>
+      <c r="L9" t="s">
+        <v>222</v>
+      </c>
+      <c r="M9" s="4" t="s">
+        <v>72</v>
+      </c>
+      <c r="O9" t="s">
+        <v>9</v>
+      </c>
+      <c r="P9" t="s">
+        <v>286</v>
+      </c>
+      <c r="Q9" s="4" t="s">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="10" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A10" s="8" t="s">
         <v>7</v>
       </c>
+      <c r="B10" t="s">
+        <v>327</v>
+      </c>
       <c r="C10" t="s">
-        <v>10</v>
+        <v>327</v>
       </c>
       <c r="D10" t="s">
-        <v>137</v>
-      </c>
-      <c r="E10" s="4" t="s">
-        <v>73</v>
+        <v>327</v>
+      </c>
+      <c r="F10" s="6" t="s">
+        <v>7</v>
       </c>
       <c r="G10" t="s">
         <v>10</v>
       </c>
       <c r="H10" t="s">
-        <v>225</v>
+        <v>137</v>
       </c>
       <c r="I10" s="4" t="s">
         <v>73</v>
       </c>
-    </row>
-    <row r="11" spans="2:10" x14ac:dyDescent="0.25">
-      <c r="B11" s="6" t="s">
+      <c r="K10" t="s">
+        <v>10</v>
+      </c>
+      <c r="L10" t="s">
+        <v>223</v>
+      </c>
+      <c r="M10" s="4" t="s">
+        <v>73</v>
+      </c>
+      <c r="O10" t="s">
+        <v>10</v>
+      </c>
+      <c r="P10" t="s">
+        <v>287</v>
+      </c>
+      <c r="Q10" s="4" t="s">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="11" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A11" s="8" t="s">
         <v>7</v>
       </c>
+      <c r="B11" t="s">
+        <v>327</v>
+      </c>
       <c r="C11" t="s">
-        <v>11</v>
+        <v>327</v>
       </c>
       <c r="D11" t="s">
-        <v>138</v>
-      </c>
-      <c r="E11" s="4" t="s">
-        <v>74</v>
+        <v>327</v>
+      </c>
+      <c r="F11" s="6" t="s">
+        <v>7</v>
       </c>
       <c r="G11" t="s">
         <v>11</v>
       </c>
       <c r="H11" t="s">
-        <v>226</v>
+        <v>138</v>
       </c>
       <c r="I11" s="4" t="s">
         <v>74</v>
       </c>
-    </row>
-    <row r="12" spans="2:10" x14ac:dyDescent="0.25">
-      <c r="B12" s="6" t="s">
+      <c r="K11" t="s">
+        <v>11</v>
+      </c>
+      <c r="L11" t="s">
+        <v>224</v>
+      </c>
+      <c r="M11" s="4" t="s">
+        <v>74</v>
+      </c>
+      <c r="O11" t="s">
+        <v>11</v>
+      </c>
+      <c r="P11" t="s">
+        <v>288</v>
+      </c>
+      <c r="Q11" s="4" t="s">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="12" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A12" s="8" t="s">
         <v>7</v>
       </c>
+      <c r="B12" t="s">
+        <v>327</v>
+      </c>
       <c r="C12" t="s">
-        <v>12</v>
+        <v>327</v>
       </c>
       <c r="D12" t="s">
-        <v>139</v>
-      </c>
-      <c r="E12" s="4" t="s">
-        <v>75</v>
+        <v>327</v>
+      </c>
+      <c r="F12" s="6" t="s">
+        <v>7</v>
       </c>
       <c r="G12" t="s">
         <v>12</v>
       </c>
       <c r="H12" t="s">
-        <v>227</v>
+        <v>139</v>
       </c>
       <c r="I12" s="4" t="s">
         <v>75</v>
       </c>
-    </row>
-    <row r="13" spans="2:10" x14ac:dyDescent="0.25">
-      <c r="B13" s="6" t="s">
+      <c r="K12" t="s">
+        <v>12</v>
+      </c>
+      <c r="L12" t="s">
+        <v>225</v>
+      </c>
+      <c r="M12" s="4" t="s">
+        <v>75</v>
+      </c>
+      <c r="O12" t="s">
+        <v>12</v>
+      </c>
+      <c r="P12" t="s">
+        <v>289</v>
+      </c>
+      <c r="Q12" s="4" t="s">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="13" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A13" s="8" t="s">
         <v>13</v>
       </c>
+      <c r="B13" t="s">
+        <v>327</v>
+      </c>
       <c r="C13" t="s">
+        <v>327</v>
+      </c>
+      <c r="D13" t="s">
+        <v>327</v>
+      </c>
+      <c r="F13" s="6" t="s">
+        <v>13</v>
+      </c>
+      <c r="G13" t="s">
         <v>14</v>
       </c>
-      <c r="D13" t="s">
+      <c r="H13" t="s">
         <v>140</v>
-      </c>
-      <c r="E13" s="4" t="s">
-        <v>76</v>
-      </c>
-      <c r="H13" t="s">
-        <v>228</v>
       </c>
       <c r="I13" s="4" t="s">
         <v>76</v>
       </c>
-    </row>
-    <row r="14" spans="2:10" x14ac:dyDescent="0.25">
+      <c r="L13" t="s">
+        <v>226</v>
+      </c>
+      <c r="M13" s="4" t="s">
+        <v>76</v>
+      </c>
+      <c r="O13" t="s">
+        <v>14</v>
+      </c>
+      <c r="P13" t="s">
+        <v>290</v>
+      </c>
+      <c r="Q13" s="4" t="s">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="14" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A14" s="6" t="s">
+        <v>13</v>
+      </c>
       <c r="B14" t="s">
+        <v>327</v>
+      </c>
+      <c r="D14" t="s">
+        <v>327</v>
+      </c>
+      <c r="F14" s="6" t="s">
         <v>13</v>
       </c>
-      <c r="C14" t="s">
+      <c r="G14" t="s">
         <v>69</v>
       </c>
-      <c r="D14" t="s">
+      <c r="H14" t="s">
         <v>141</v>
       </c>
-      <c r="E14" s="4" t="s">
+      <c r="I14" s="4" t="s">
         <v>77</v>
       </c>
-    </row>
-    <row r="15" spans="2:10" x14ac:dyDescent="0.25">
-      <c r="B15" s="6" t="s">
+      <c r="O14" t="s">
+        <v>69</v>
+      </c>
+      <c r="P14" t="s">
+        <v>291</v>
+      </c>
+      <c r="Q14" s="4" t="s">
+        <v>77</v>
+      </c>
+    </row>
+    <row r="15" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A15" s="8" t="s">
         <v>129</v>
       </c>
+      <c r="B15" t="s">
+        <v>327</v>
+      </c>
       <c r="C15" t="s">
-        <v>70</v>
+        <v>327</v>
       </c>
       <c r="D15" t="s">
-        <v>142</v>
-      </c>
-      <c r="E15" s="4" t="s">
-        <v>78</v>
+        <v>327</v>
+      </c>
+      <c r="F15" s="6" t="s">
+        <v>129</v>
       </c>
       <c r="G15" t="s">
         <v>70</v>
       </c>
       <c r="H15" t="s">
-        <v>229</v>
+        <v>142</v>
       </c>
       <c r="I15" s="4" t="s">
         <v>78</v>
       </c>
-    </row>
-    <row r="16" spans="2:10" x14ac:dyDescent="0.25">
-      <c r="B16" s="6" t="s">
+      <c r="K15" t="s">
+        <v>70</v>
+      </c>
+      <c r="L15" t="s">
+        <v>227</v>
+      </c>
+      <c r="M15" s="4" t="s">
+        <v>78</v>
+      </c>
+      <c r="O15" t="s">
+        <v>70</v>
+      </c>
+      <c r="P15" t="s">
+        <v>292</v>
+      </c>
+      <c r="Q15" s="4" t="s">
+        <v>78</v>
+      </c>
+    </row>
+    <row r="16" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A16" s="8" t="s">
         <v>129</v>
       </c>
+      <c r="B16" t="s">
+        <v>327</v>
+      </c>
       <c r="C16" t="s">
+        <v>327</v>
+      </c>
+      <c r="D16" t="s">
+        <v>327</v>
+      </c>
+      <c r="F16" s="6" t="s">
+        <v>129</v>
+      </c>
+      <c r="G16" t="s">
         <v>15</v>
       </c>
-      <c r="D16" t="s">
+      <c r="H16" t="s">
         <v>143</v>
-      </c>
-      <c r="E16" s="4" t="s">
-        <v>15</v>
-      </c>
-      <c r="G16" t="s">
-        <v>208</v>
-      </c>
-      <c r="H16" t="s">
-        <v>230</v>
       </c>
       <c r="I16" s="4" t="s">
         <v>15</v>
       </c>
-    </row>
-    <row r="17" spans="2:9" x14ac:dyDescent="0.25">
-      <c r="B17" s="6" t="s">
+      <c r="K16" t="s">
+        <v>207</v>
+      </c>
+      <c r="L16" t="s">
+        <v>228</v>
+      </c>
+      <c r="M16" s="4" t="s">
+        <v>15</v>
+      </c>
+      <c r="O16" t="s">
+        <v>207</v>
+      </c>
+      <c r="P16" t="s">
+        <v>293</v>
+      </c>
+      <c r="Q16" s="4" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="17" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A17" s="8" t="s">
         <v>129</v>
       </c>
+      <c r="B17" t="s">
+        <v>327</v>
+      </c>
       <c r="C17" t="s">
-        <v>16</v>
+        <v>327</v>
       </c>
       <c r="D17" t="s">
-        <v>144</v>
-      </c>
-      <c r="E17" s="4" t="s">
-        <v>79</v>
+        <v>327</v>
+      </c>
+      <c r="F17" s="6" t="s">
+        <v>129</v>
       </c>
       <c r="G17" t="s">
         <v>16</v>
       </c>
       <c r="H17" t="s">
-        <v>231</v>
+        <v>144</v>
       </c>
       <c r="I17" s="4" t="s">
         <v>79</v>
       </c>
-    </row>
-    <row r="18" spans="2:9" x14ac:dyDescent="0.25">
-      <c r="B18" s="6" t="s">
+      <c r="K17" t="s">
+        <v>16</v>
+      </c>
+      <c r="L17" t="s">
+        <v>229</v>
+      </c>
+      <c r="M17" s="4" t="s">
+        <v>79</v>
+      </c>
+      <c r="O17" t="s">
+        <v>16</v>
+      </c>
+      <c r="P17" t="s">
+        <v>294</v>
+      </c>
+      <c r="Q17" s="4" t="s">
+        <v>79</v>
+      </c>
+    </row>
+    <row r="18" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A18" s="8" t="s">
         <v>17</v>
       </c>
+      <c r="B18" t="s">
+        <v>327</v>
+      </c>
       <c r="C18" t="s">
+        <v>327</v>
+      </c>
+      <c r="D18" t="s">
+        <v>327</v>
+      </c>
+      <c r="F18" s="6" t="s">
+        <v>17</v>
+      </c>
+      <c r="G18" t="s">
         <v>18</v>
       </c>
-      <c r="D18" t="s">
+      <c r="H18" t="s">
         <v>145</v>
-      </c>
-      <c r="E18" s="4" t="s">
-        <v>80</v>
-      </c>
-      <c r="G18" t="s">
-        <v>209</v>
-      </c>
-      <c r="H18" t="s">
-        <v>232</v>
       </c>
       <c r="I18" s="4" t="s">
         <v>80</v>
       </c>
-    </row>
-    <row r="19" spans="2:9" ht="30" x14ac:dyDescent="0.25">
-      <c r="B19" s="6" t="s">
+      <c r="K18" t="s">
+        <v>208</v>
+      </c>
+      <c r="L18" t="s">
+        <v>230</v>
+      </c>
+      <c r="M18" s="4" t="s">
+        <v>80</v>
+      </c>
+      <c r="O18" t="s">
+        <v>208</v>
+      </c>
+      <c r="P18" t="s">
+        <v>295</v>
+      </c>
+      <c r="Q18" s="4" t="s">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="19" spans="1:17" ht="45" x14ac:dyDescent="0.25">
+      <c r="A19" s="8" t="s">
         <v>17</v>
       </c>
+      <c r="B19" t="s">
+        <v>327</v>
+      </c>
       <c r="C19" t="s">
-        <v>66</v>
+        <v>327</v>
       </c>
       <c r="D19" t="s">
-        <v>146</v>
-      </c>
-      <c r="E19" s="4" t="s">
-        <v>115</v>
+        <v>327</v>
+      </c>
+      <c r="F19" s="6" t="s">
+        <v>17</v>
       </c>
       <c r="G19" t="s">
         <v>66</v>
       </c>
       <c r="H19" t="s">
-        <v>233</v>
+        <v>146</v>
       </c>
       <c r="I19" s="4" t="s">
         <v>115</v>
       </c>
-    </row>
-    <row r="20" spans="2:9" ht="30" x14ac:dyDescent="0.25">
+      <c r="K19" t="s">
+        <v>66</v>
+      </c>
+      <c r="L19" t="s">
+        <v>231</v>
+      </c>
+      <c r="M19" s="4" t="s">
+        <v>115</v>
+      </c>
+      <c r="O19" t="s">
+        <v>66</v>
+      </c>
+      <c r="P19" t="s">
+        <v>296</v>
+      </c>
+      <c r="Q19" s="4" t="s">
+        <v>115</v>
+      </c>
+    </row>
+    <row r="20" spans="1:17" ht="30" x14ac:dyDescent="0.25">
+      <c r="A20" s="6" t="s">
+        <v>19</v>
+      </c>
       <c r="B20" t="s">
+        <v>327</v>
+      </c>
+      <c r="F20" s="6" t="s">
         <v>19</v>
       </c>
-      <c r="C20" t="s">
+      <c r="G20" t="s">
         <v>37</v>
       </c>
-      <c r="D20" t="s">
+      <c r="H20" t="s">
         <v>147</v>
       </c>
-      <c r="E20" s="4" t="s">
+      <c r="I20" s="4" t="s">
         <v>81</v>
       </c>
     </row>
-    <row r="21" spans="2:9" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A21" s="6" t="s">
+        <v>19</v>
+      </c>
       <c r="B21" t="s">
+        <v>327</v>
+      </c>
+      <c r="F21" s="6" t="s">
         <v>19</v>
       </c>
-      <c r="C21" t="s">
+      <c r="G21" t="s">
         <v>38</v>
       </c>
-      <c r="D21" t="s">
+      <c r="H21" t="s">
         <v>148</v>
       </c>
-      <c r="E21" s="4" t="s">
+      <c r="I21" s="4" t="s">
         <v>82</v>
       </c>
     </row>
-    <row r="22" spans="2:9" ht="30" x14ac:dyDescent="0.25">
-      <c r="B22" s="6" t="s">
+    <row r="22" spans="1:17" ht="45" x14ac:dyDescent="0.25">
+      <c r="A22" s="8" t="s">
         <v>19</v>
       </c>
+      <c r="B22" t="s">
+        <v>327</v>
+      </c>
       <c r="C22" t="s">
+        <v>327</v>
+      </c>
+      <c r="D22" t="s">
+        <v>327</v>
+      </c>
+      <c r="F22" s="6" t="s">
+        <v>19</v>
+      </c>
+      <c r="G22" t="s">
         <v>39</v>
       </c>
-      <c r="D22" t="s">
+      <c r="H22" t="s">
         <v>149</v>
-      </c>
-      <c r="E22" s="4" t="s">
-        <v>83</v>
-      </c>
-      <c r="G22" t="s">
-        <v>190</v>
-      </c>
-      <c r="H22" t="s">
-        <v>234</v>
       </c>
       <c r="I22" s="4" t="s">
         <v>83</v>
       </c>
-    </row>
-    <row r="23" spans="2:9" ht="30" x14ac:dyDescent="0.25">
-      <c r="B23" s="6" t="s">
+      <c r="K22" t="s">
+        <v>190</v>
+      </c>
+      <c r="L22" t="s">
+        <v>232</v>
+      </c>
+      <c r="M22" s="4" t="s">
+        <v>83</v>
+      </c>
+      <c r="O22" t="s">
+        <v>265</v>
+      </c>
+      <c r="P22" t="s">
+        <v>297</v>
+      </c>
+      <c r="Q22" s="4" t="s">
+        <v>83</v>
+      </c>
+    </row>
+    <row r="23" spans="1:17" ht="60" x14ac:dyDescent="0.25">
+      <c r="A23" s="8" t="s">
         <v>19</v>
       </c>
+      <c r="B23" t="s">
+        <v>327</v>
+      </c>
       <c r="C23" t="s">
+        <v>327</v>
+      </c>
+      <c r="D23" t="s">
+        <v>327</v>
+      </c>
+      <c r="F23" s="6" t="s">
+        <v>19</v>
+      </c>
+      <c r="G23" t="s">
         <v>40</v>
       </c>
-      <c r="D23" t="s">
+      <c r="H23" t="s">
         <v>150</v>
-      </c>
-      <c r="E23" s="4" t="s">
-        <v>84</v>
-      </c>
-      <c r="G23" t="s">
-        <v>191</v>
-      </c>
-      <c r="H23" t="s">
-        <v>235</v>
       </c>
       <c r="I23" s="4" t="s">
         <v>84</v>
       </c>
-    </row>
-    <row r="24" spans="2:9" x14ac:dyDescent="0.25">
-      <c r="B24" s="6" t="s">
+      <c r="K23" t="s">
+        <v>191</v>
+      </c>
+      <c r="L23" t="s">
+        <v>233</v>
+      </c>
+      <c r="M23" s="4" t="s">
+        <v>84</v>
+      </c>
+      <c r="O23" t="s">
+        <v>266</v>
+      </c>
+      <c r="P23" t="s">
+        <v>298</v>
+      </c>
+      <c r="Q23" s="4" t="s">
+        <v>84</v>
+      </c>
+    </row>
+    <row r="24" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A24" s="8" t="s">
         <v>19</v>
       </c>
+      <c r="B24" t="s">
+        <v>327</v>
+      </c>
       <c r="C24" t="s">
+        <v>327</v>
+      </c>
+      <c r="D24" t="s">
+        <v>327</v>
+      </c>
+      <c r="F24" s="6" t="s">
+        <v>19</v>
+      </c>
+      <c r="G24" t="s">
         <v>41</v>
       </c>
-      <c r="D24" t="s">
+      <c r="H24" t="s">
         <v>151</v>
-      </c>
-      <c r="E24" s="4" t="s">
-        <v>85</v>
-      </c>
-      <c r="G24" t="s">
-        <v>192</v>
-      </c>
-      <c r="H24" t="s">
-        <v>236</v>
       </c>
       <c r="I24" s="4" t="s">
         <v>85</v>
       </c>
-    </row>
-    <row r="25" spans="2:9" ht="30" x14ac:dyDescent="0.25">
-      <c r="B25" s="6" t="s">
+      <c r="K24" t="s">
+        <v>192</v>
+      </c>
+      <c r="L24" t="s">
+        <v>234</v>
+      </c>
+      <c r="M24" s="4" t="s">
+        <v>85</v>
+      </c>
+      <c r="O24" t="s">
+        <v>267</v>
+      </c>
+      <c r="P24" t="s">
+        <v>299</v>
+      </c>
+      <c r="Q24" s="4" t="s">
+        <v>85</v>
+      </c>
+    </row>
+    <row r="25" spans="1:17" ht="30" x14ac:dyDescent="0.25">
+      <c r="A25" s="8" t="s">
         <v>19</v>
       </c>
+      <c r="B25" t="s">
+        <v>327</v>
+      </c>
       <c r="C25" t="s">
+        <v>327</v>
+      </c>
+      <c r="D25" t="s">
+        <v>327</v>
+      </c>
+      <c r="F25" s="6" t="s">
+        <v>19</v>
+      </c>
+      <c r="G25" t="s">
         <v>42</v>
       </c>
-      <c r="D25" t="s">
+      <c r="H25" t="s">
         <v>152</v>
-      </c>
-      <c r="E25" s="4" t="s">
-        <v>86</v>
-      </c>
-      <c r="G25" t="s">
-        <v>193</v>
-      </c>
-      <c r="H25" t="s">
-        <v>237</v>
       </c>
       <c r="I25" s="4" t="s">
         <v>86</v>
       </c>
-    </row>
-    <row r="26" spans="2:9" ht="30" x14ac:dyDescent="0.25">
+      <c r="K25" t="s">
+        <v>193</v>
+      </c>
+      <c r="L25" t="s">
+        <v>235</v>
+      </c>
+      <c r="M25" s="4" t="s">
+        <v>86</v>
+      </c>
+      <c r="O25" t="s">
+        <v>268</v>
+      </c>
+      <c r="P25" t="s">
+        <v>300</v>
+      </c>
+      <c r="Q25" s="4" t="s">
+        <v>86</v>
+      </c>
+    </row>
+    <row r="26" spans="1:17" ht="45" x14ac:dyDescent="0.25">
+      <c r="A26" s="6" t="s">
+        <v>19</v>
+      </c>
       <c r="B26" t="s">
+        <v>327</v>
+      </c>
+      <c r="F26" s="6" t="s">
         <v>19</v>
       </c>
-      <c r="C26" t="s">
+      <c r="G26" t="s">
         <v>43</v>
       </c>
-      <c r="D26" t="s">
+      <c r="H26" t="s">
         <v>153</v>
       </c>
-      <c r="E26" s="4" t="s">
+      <c r="I26" s="4" t="s">
         <v>101</v>
       </c>
     </row>
-    <row r="27" spans="2:9" ht="30" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:17" ht="45" x14ac:dyDescent="0.25">
+      <c r="A27" s="6" t="s">
+        <v>19</v>
+      </c>
       <c r="B27" t="s">
+        <v>327</v>
+      </c>
+      <c r="F27" s="6" t="s">
         <v>19</v>
       </c>
-      <c r="C27" t="s">
+      <c r="G27" t="s">
         <v>44</v>
       </c>
-      <c r="D27" t="s">
+      <c r="H27" t="s">
         <v>154</v>
       </c>
-      <c r="E27" s="4" t="s">
+      <c r="I27" s="4" t="s">
         <v>102</v>
       </c>
     </row>
-    <row r="28" spans="2:9" ht="45" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:17" ht="60" x14ac:dyDescent="0.25">
+      <c r="A28" s="6" t="s">
+        <v>19</v>
+      </c>
       <c r="B28" t="s">
+        <v>327</v>
+      </c>
+      <c r="F28" s="6" t="s">
         <v>19</v>
       </c>
-      <c r="C28" t="s">
+      <c r="G28" t="s">
         <v>45</v>
       </c>
-      <c r="D28" t="s">
+      <c r="H28" t="s">
         <v>155</v>
       </c>
-      <c r="E28" s="4" t="s">
+      <c r="I28" s="4" t="s">
         <v>103</v>
       </c>
     </row>
-    <row r="29" spans="2:9" ht="45" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:17" ht="60" x14ac:dyDescent="0.25">
+      <c r="A29" s="6" t="s">
+        <v>19</v>
+      </c>
       <c r="B29" t="s">
+        <v>327</v>
+      </c>
+      <c r="F29" s="6" t="s">
         <v>19</v>
       </c>
-      <c r="C29" t="s">
+      <c r="G29" t="s">
         <v>46</v>
       </c>
-      <c r="D29" t="s">
+      <c r="H29" t="s">
         <v>156</v>
       </c>
-      <c r="E29" s="4" t="s">
+      <c r="I29" s="4" t="s">
         <v>104</v>
       </c>
     </row>
-    <row r="30" spans="2:9" ht="60" x14ac:dyDescent="0.25">
-      <c r="B30" s="6" t="s">
+    <row r="30" spans="1:17" ht="75" x14ac:dyDescent="0.25">
+      <c r="A30" s="6" t="s">
         <v>20</v>
       </c>
+      <c r="B30" t="s">
+        <v>327</v>
+      </c>
       <c r="C30" t="s">
+        <v>327</v>
+      </c>
+      <c r="D30" t="s">
+        <v>327</v>
+      </c>
+      <c r="F30" s="6" t="s">
+        <v>20</v>
+      </c>
+      <c r="G30" t="s">
         <v>47</v>
       </c>
-      <c r="D30" t="s">
+      <c r="H30" t="s">
         <v>157</v>
-      </c>
-      <c r="E30" s="4" t="s">
-        <v>87</v>
-      </c>
-      <c r="G30" t="s">
-        <v>194</v>
-      </c>
-      <c r="H30" t="s">
-        <v>238</v>
       </c>
       <c r="I30" s="4" t="s">
         <v>87</v>
       </c>
-    </row>
-    <row r="31" spans="2:9" ht="30" x14ac:dyDescent="0.25">
-      <c r="B31" s="6" t="s">
+      <c r="K30" t="s">
+        <v>194</v>
+      </c>
+      <c r="L30" t="s">
+        <v>236</v>
+      </c>
+      <c r="M30" s="4" t="s">
+        <v>87</v>
+      </c>
+      <c r="O30" t="s">
+        <v>269</v>
+      </c>
+      <c r="P30" t="s">
+        <v>301</v>
+      </c>
+      <c r="Q30" s="4" t="s">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="31" spans="1:17" ht="45" x14ac:dyDescent="0.25">
+      <c r="A31" s="8" t="s">
         <v>20</v>
       </c>
+      <c r="B31" t="s">
+        <v>327</v>
+      </c>
       <c r="C31" t="s">
+        <v>327</v>
+      </c>
+      <c r="D31" t="s">
+        <v>327</v>
+      </c>
+      <c r="F31" s="6" t="s">
+        <v>20</v>
+      </c>
+      <c r="G31" t="s">
         <v>48</v>
       </c>
-      <c r="D31" t="s">
+      <c r="H31" t="s">
         <v>158</v>
-      </c>
-      <c r="E31" s="4" t="s">
-        <v>88</v>
-      </c>
-      <c r="G31" t="s">
-        <v>195</v>
-      </c>
-      <c r="H31" t="s">
-        <v>239</v>
       </c>
       <c r="I31" s="4" t="s">
         <v>88</v>
       </c>
-    </row>
-    <row r="32" spans="2:9" ht="45" x14ac:dyDescent="0.25">
-      <c r="B32" s="6" t="s">
+      <c r="K31" t="s">
+        <v>195</v>
+      </c>
+      <c r="L31" t="s">
+        <v>237</v>
+      </c>
+      <c r="M31" s="4" t="s">
+        <v>88</v>
+      </c>
+      <c r="O31" t="s">
+        <v>270</v>
+      </c>
+      <c r="P31" t="s">
+        <v>302</v>
+      </c>
+      <c r="Q31" s="4" t="s">
+        <v>88</v>
+      </c>
+    </row>
+    <row r="32" spans="1:17" ht="60" x14ac:dyDescent="0.25">
+      <c r="A32" s="6" t="s">
         <v>20</v>
       </c>
-      <c r="C32" t="s">
+      <c r="B32" t="s">
+        <v>327</v>
+      </c>
+      <c r="F32" s="6" t="s">
+        <v>20</v>
+      </c>
+      <c r="G32" t="s">
         <v>49</v>
       </c>
-      <c r="D32" t="s">
+      <c r="H32" t="s">
         <v>159</v>
       </c>
-      <c r="E32" s="4" t="s">
+      <c r="I32" s="4" t="s">
         <v>89</v>
       </c>
     </row>
-    <row r="33" spans="2:18" ht="30" x14ac:dyDescent="0.25">
-      <c r="B33" s="6" t="s">
+    <row r="33" spans="1:22" ht="45" x14ac:dyDescent="0.25">
+      <c r="A33" s="8" t="s">
         <v>20</v>
       </c>
+      <c r="B33" t="s">
+        <v>327</v>
+      </c>
       <c r="C33" t="s">
+        <v>327</v>
+      </c>
+      <c r="D33" t="s">
+        <v>327</v>
+      </c>
+      <c r="F33" s="6" t="s">
+        <v>20</v>
+      </c>
+      <c r="G33" t="s">
         <v>50</v>
       </c>
-      <c r="D33" t="s">
+      <c r="H33" t="s">
         <v>160</v>
-      </c>
-      <c r="E33" s="4" t="s">
-        <v>90</v>
-      </c>
-      <c r="G33" t="s">
-        <v>197</v>
-      </c>
-      <c r="H33" t="s">
-        <v>240</v>
       </c>
       <c r="I33" s="4" t="s">
         <v>90</v>
       </c>
-      <c r="Q33" t="s">
-        <v>207</v>
-      </c>
-      <c r="R33" t="s">
-        <v>216</v>
-      </c>
-    </row>
-    <row r="34" spans="2:18" ht="30" x14ac:dyDescent="0.25">
-      <c r="B34" s="6" t="s">
+      <c r="K33" t="s">
+        <v>196</v>
+      </c>
+      <c r="L33" t="s">
+        <v>238</v>
+      </c>
+      <c r="M33" s="4" t="s">
+        <v>90</v>
+      </c>
+      <c r="O33" t="s">
+        <v>271</v>
+      </c>
+      <c r="P33" t="s">
+        <v>303</v>
+      </c>
+      <c r="Q33" s="4" t="s">
+        <v>90</v>
+      </c>
+      <c r="U33" t="s">
+        <v>206</v>
+      </c>
+      <c r="V33" t="s">
+        <v>214</v>
+      </c>
+    </row>
+    <row r="34" spans="1:22" ht="45" x14ac:dyDescent="0.25">
+      <c r="A34" s="8" t="s">
         <v>20</v>
       </c>
+      <c r="B34" t="s">
+        <v>327</v>
+      </c>
       <c r="C34" t="s">
+        <v>327</v>
+      </c>
+      <c r="D34" t="s">
+        <v>327</v>
+      </c>
+      <c r="F34" s="6" t="s">
+        <v>20</v>
+      </c>
+      <c r="G34" t="s">
         <v>51</v>
       </c>
-      <c r="D34" t="s">
+      <c r="H34" t="s">
         <v>161</v>
-      </c>
-      <c r="E34" s="4" t="s">
-        <v>91</v>
-      </c>
-      <c r="G34" t="s">
-        <v>199</v>
-      </c>
-      <c r="H34" t="s">
-        <v>241</v>
       </c>
       <c r="I34" s="4" t="s">
         <v>91</v>
       </c>
-    </row>
-    <row r="35" spans="2:18" x14ac:dyDescent="0.25">
-      <c r="B35" s="6" t="s">
+      <c r="K34" t="s">
+        <v>198</v>
+      </c>
+      <c r="L34" t="s">
+        <v>239</v>
+      </c>
+      <c r="M34" s="4" t="s">
+        <v>91</v>
+      </c>
+    </row>
+    <row r="35" spans="1:22" ht="30" x14ac:dyDescent="0.25">
+      <c r="A35" s="8" t="s">
         <v>20</v>
       </c>
+      <c r="B35" t="s">
+        <v>327</v>
+      </c>
       <c r="C35" t="s">
+        <v>327</v>
+      </c>
+      <c r="D35" t="s">
+        <v>327</v>
+      </c>
+      <c r="F35" s="6" t="s">
+        <v>20</v>
+      </c>
+      <c r="G35" t="s">
         <v>52</v>
       </c>
-      <c r="D35" t="s">
+      <c r="H35" t="s">
         <v>162</v>
-      </c>
-      <c r="E35" s="4" t="s">
-        <v>92</v>
-      </c>
-      <c r="G35" t="s">
-        <v>198</v>
-      </c>
-      <c r="H35" t="s">
-        <v>242</v>
       </c>
       <c r="I35" s="4" t="s">
         <v>92</v>
       </c>
-    </row>
-    <row r="36" spans="2:18" ht="30" x14ac:dyDescent="0.25">
-      <c r="B36" s="6" t="s">
+      <c r="K35" t="s">
+        <v>197</v>
+      </c>
+      <c r="L35" t="s">
+        <v>240</v>
+      </c>
+      <c r="M35" s="4" t="s">
+        <v>92</v>
+      </c>
+      <c r="O35" t="s">
+        <v>272</v>
+      </c>
+      <c r="P35" t="s">
+        <v>304</v>
+      </c>
+      <c r="Q35" s="4" t="s">
+        <v>92</v>
+      </c>
+    </row>
+    <row r="36" spans="1:22" ht="30" x14ac:dyDescent="0.25">
+      <c r="A36" s="6" t="s">
         <v>20</v>
       </c>
-      <c r="C36" t="s">
+      <c r="B36" t="s">
+        <v>327</v>
+      </c>
+      <c r="F36" s="6" t="s">
+        <v>20</v>
+      </c>
+      <c r="G36" t="s">
         <v>53</v>
       </c>
-      <c r="D36" t="s">
+      <c r="H36" t="s">
         <v>163</v>
       </c>
-      <c r="E36" s="4" t="s">
+      <c r="I36" s="4" t="s">
         <v>93</v>
       </c>
     </row>
-    <row r="37" spans="2:18" x14ac:dyDescent="0.25">
-      <c r="B37" s="6" t="s">
+    <row r="37" spans="1:22" x14ac:dyDescent="0.25">
+      <c r="A37" s="6" t="s">
         <v>20</v>
       </c>
-      <c r="C37" t="s">
+      <c r="B37" t="s">
+        <v>327</v>
+      </c>
+      <c r="D37" t="s">
+        <v>327</v>
+      </c>
+      <c r="F37" s="6" t="s">
+        <v>20</v>
+      </c>
+      <c r="G37" t="s">
         <v>54</v>
       </c>
-      <c r="D37" t="s">
+      <c r="H37" t="s">
         <v>164</v>
       </c>
-      <c r="E37" s="4" t="s">
+      <c r="I37" s="4" t="s">
         <v>94</v>
       </c>
-    </row>
-    <row r="38" spans="2:18" x14ac:dyDescent="0.25">
+      <c r="O37" t="s">
+        <v>273</v>
+      </c>
+      <c r="P37" t="s">
+        <v>305</v>
+      </c>
+      <c r="Q37" s="4" t="s">
+        <v>94</v>
+      </c>
+    </row>
+    <row r="38" spans="1:22" ht="30" x14ac:dyDescent="0.25">
+      <c r="A38" s="8" t="s">
+        <v>21</v>
+      </c>
+      <c r="B38" t="s">
+        <v>327</v>
+      </c>
+      <c r="C38" t="s">
+        <v>327</v>
+      </c>
+      <c r="D38" t="s">
+        <v>327</v>
+      </c>
+      <c r="F38" s="6" t="s">
+        <v>21</v>
+      </c>
       <c r="G38" t="s">
-        <v>196</v>
+        <v>55</v>
+      </c>
+      <c r="H38" t="s">
+        <v>165</v>
       </c>
       <c r="I38" s="4" t="s">
-        <v>214</v>
-      </c>
-    </row>
-    <row r="40" spans="2:18" ht="30" x14ac:dyDescent="0.25">
-      <c r="B40" s="6" t="s">
+        <v>95</v>
+      </c>
+      <c r="K38" t="s">
+        <v>199</v>
+      </c>
+      <c r="L38" t="s">
+        <v>241</v>
+      </c>
+      <c r="M38" s="4" t="s">
+        <v>95</v>
+      </c>
+      <c r="O38" t="s">
+        <v>274</v>
+      </c>
+      <c r="P38" t="s">
+        <v>306</v>
+      </c>
+      <c r="Q38" s="4" t="s">
+        <v>95</v>
+      </c>
+    </row>
+    <row r="39" spans="1:22" ht="45" x14ac:dyDescent="0.25">
+      <c r="A39" s="8" t="s">
         <v>21</v>
       </c>
+      <c r="B39" t="s">
+        <v>327</v>
+      </c>
+      <c r="C39" t="s">
+        <v>327</v>
+      </c>
+      <c r="D39" t="s">
+        <v>327</v>
+      </c>
+      <c r="F39" s="6" t="s">
+        <v>21</v>
+      </c>
+      <c r="G39" t="s">
+        <v>56</v>
+      </c>
+      <c r="H39" t="s">
+        <v>166</v>
+      </c>
+      <c r="I39" s="4" t="s">
+        <v>96</v>
+      </c>
+      <c r="K39" t="s">
+        <v>200</v>
+      </c>
+      <c r="L39" t="s">
+        <v>242</v>
+      </c>
+      <c r="M39" s="4" t="s">
+        <v>96</v>
+      </c>
+      <c r="O39" t="s">
+        <v>275</v>
+      </c>
+      <c r="P39" t="s">
+        <v>307</v>
+      </c>
+      <c r="Q39" s="4" t="s">
+        <v>96</v>
+      </c>
+    </row>
+    <row r="40" spans="1:22" ht="30" x14ac:dyDescent="0.25">
+      <c r="A40" s="8" t="s">
+        <v>21</v>
+      </c>
+      <c r="B40" t="s">
+        <v>327</v>
+      </c>
       <c r="C40" t="s">
-        <v>55</v>
+        <v>327</v>
       </c>
       <c r="D40" t="s">
-        <v>165</v>
-      </c>
-      <c r="E40" s="4" t="s">
-        <v>95</v>
+        <v>327</v>
+      </c>
+      <c r="F40" s="6" t="s">
+        <v>21</v>
       </c>
       <c r="G40" t="s">
-        <v>200</v>
+        <v>57</v>
       </c>
       <c r="H40" t="s">
+        <v>167</v>
+      </c>
+      <c r="I40" s="4" t="s">
+        <v>97</v>
+      </c>
+      <c r="K40" t="s">
+        <v>201</v>
+      </c>
+      <c r="L40" t="s">
         <v>243</v>
       </c>
-      <c r="I40" s="4" t="s">
-        <v>95</v>
-      </c>
-    </row>
-    <row r="41" spans="2:18" ht="30" x14ac:dyDescent="0.25">
-      <c r="B41" s="6" t="s">
+      <c r="M40" s="4" t="s">
+        <v>97</v>
+      </c>
+      <c r="O40" t="s">
+        <v>276</v>
+      </c>
+      <c r="P40" t="s">
+        <v>308</v>
+      </c>
+      <c r="Q40" s="4" t="s">
+        <v>97</v>
+      </c>
+    </row>
+    <row r="41" spans="1:22" ht="45" x14ac:dyDescent="0.25">
+      <c r="A41" s="8" t="s">
         <v>21</v>
       </c>
+      <c r="B41" t="s">
+        <v>327</v>
+      </c>
       <c r="C41" t="s">
-        <v>56</v>
+        <v>327</v>
       </c>
       <c r="D41" t="s">
-        <v>166</v>
-      </c>
-      <c r="E41" s="4" t="s">
-        <v>96</v>
+        <v>327</v>
+      </c>
+      <c r="F41" s="6" t="s">
+        <v>21</v>
       </c>
       <c r="G41" t="s">
-        <v>201</v>
+        <v>58</v>
       </c>
       <c r="H41" t="s">
+        <v>168</v>
+      </c>
+      <c r="I41" s="4" t="s">
+        <v>98</v>
+      </c>
+      <c r="K41" t="s">
+        <v>202</v>
+      </c>
+      <c r="L41" t="s">
         <v>244</v>
       </c>
-      <c r="I41" s="4" t="s">
-        <v>96</v>
-      </c>
-    </row>
-    <row r="42" spans="2:18" ht="30" x14ac:dyDescent="0.25">
-      <c r="B42" s="6" t="s">
+      <c r="M41" s="4" t="s">
+        <v>98</v>
+      </c>
+      <c r="O41" t="s">
+        <v>277</v>
+      </c>
+      <c r="P41" t="s">
+        <v>309</v>
+      </c>
+      <c r="Q41" s="4" t="s">
+        <v>98</v>
+      </c>
+    </row>
+    <row r="42" spans="1:22" ht="45" x14ac:dyDescent="0.25">
+      <c r="A42" s="8" t="s">
         <v>21</v>
       </c>
+      <c r="B42" t="s">
+        <v>327</v>
+      </c>
       <c r="C42" t="s">
-        <v>57</v>
+        <v>327</v>
       </c>
       <c r="D42" t="s">
-        <v>167</v>
-      </c>
-      <c r="E42" s="4" t="s">
-        <v>97</v>
+        <v>327</v>
+      </c>
+      <c r="F42" s="6" t="s">
+        <v>21</v>
       </c>
       <c r="G42" t="s">
-        <v>202</v>
+        <v>59</v>
       </c>
       <c r="H42" t="s">
+        <v>169</v>
+      </c>
+      <c r="I42" s="4" t="s">
+        <v>99</v>
+      </c>
+      <c r="K42" t="s">
+        <v>203</v>
+      </c>
+      <c r="L42" t="s">
         <v>245</v>
       </c>
-      <c r="I42" s="4" t="s">
-        <v>97</v>
-      </c>
-    </row>
-    <row r="43" spans="2:18" ht="30" x14ac:dyDescent="0.25">
-      <c r="B43" s="6" t="s">
+      <c r="M42" s="4" t="s">
+        <v>99</v>
+      </c>
+      <c r="O42" t="s">
+        <v>278</v>
+      </c>
+      <c r="P42" t="s">
+        <v>310</v>
+      </c>
+      <c r="Q42" s="4" t="s">
+        <v>99</v>
+      </c>
+    </row>
+    <row r="43" spans="1:22" ht="30" x14ac:dyDescent="0.25">
+      <c r="A43" s="6" t="s">
         <v>21</v>
       </c>
-      <c r="C43" t="s">
-        <v>58</v>
-      </c>
-      <c r="D43" t="s">
-        <v>168</v>
-      </c>
-      <c r="E43" s="4" t="s">
-        <v>98</v>
+      <c r="B43" t="s">
+        <v>327</v>
+      </c>
+      <c r="F43" s="6" t="s">
+        <v>21</v>
       </c>
       <c r="G43" t="s">
-        <v>203</v>
+        <v>60</v>
       </c>
       <c r="H43" t="s">
+        <v>170</v>
+      </c>
+      <c r="I43" s="4" t="s">
+        <v>100</v>
+      </c>
+      <c r="K43" t="s">
+        <v>204</v>
+      </c>
+      <c r="L43" t="s">
         <v>246</v>
       </c>
-      <c r="I43" s="4" t="s">
-        <v>98</v>
-      </c>
-    </row>
-    <row r="44" spans="2:18" ht="30" x14ac:dyDescent="0.25">
-      <c r="B44" s="6" t="s">
-        <v>21</v>
+      <c r="M43" s="4" t="s">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="44" spans="1:22" ht="45" x14ac:dyDescent="0.25">
+      <c r="A44" s="8" t="s">
+        <v>22</v>
+      </c>
+      <c r="B44" t="s">
+        <v>327</v>
       </c>
       <c r="C44" t="s">
-        <v>59</v>
+        <v>327</v>
       </c>
       <c r="D44" t="s">
-        <v>169</v>
-      </c>
-      <c r="E44" s="4" t="s">
-        <v>99</v>
+        <v>327</v>
+      </c>
+      <c r="F44" s="6" t="s">
+        <v>22</v>
       </c>
       <c r="G44" t="s">
-        <v>204</v>
+        <v>61</v>
       </c>
       <c r="H44" t="s">
+        <v>171</v>
+      </c>
+      <c r="I44" s="4" t="s">
+        <v>213</v>
+      </c>
+      <c r="K44" t="s">
+        <v>205</v>
+      </c>
+      <c r="L44" t="s">
         <v>247</v>
       </c>
-      <c r="I44" s="4" t="s">
-        <v>99</v>
-      </c>
-    </row>
-    <row r="45" spans="2:18" x14ac:dyDescent="0.25">
-      <c r="B45" s="6" t="s">
-        <v>21</v>
+      <c r="M44" s="4" t="s">
+        <v>213</v>
+      </c>
+      <c r="O44" t="s">
+        <v>279</v>
+      </c>
+      <c r="P44" t="s">
+        <v>311</v>
+      </c>
+      <c r="Q44" s="4" t="s">
+        <v>213</v>
+      </c>
+    </row>
+    <row r="45" spans="1:22" x14ac:dyDescent="0.25">
+      <c r="A45" s="8" t="s">
+        <v>23</v>
+      </c>
+      <c r="B45" t="s">
+        <v>327</v>
       </c>
       <c r="C45" t="s">
-        <v>60</v>
+        <v>327</v>
       </c>
       <c r="D45" t="s">
-        <v>170</v>
-      </c>
-      <c r="E45" s="4" t="s">
-        <v>100</v>
+        <v>327</v>
+      </c>
+      <c r="F45" s="6" t="s">
+        <v>23</v>
       </c>
       <c r="G45" t="s">
-        <v>205</v>
+        <v>24</v>
       </c>
       <c r="H45" t="s">
+        <v>172</v>
+      </c>
+      <c r="I45" s="4" t="s">
+        <v>110</v>
+      </c>
+      <c r="K45" t="s">
+        <v>24</v>
+      </c>
+      <c r="L45" t="s">
         <v>248</v>
       </c>
-      <c r="I45" s="4" t="s">
-        <v>100</v>
-      </c>
-    </row>
-    <row r="46" spans="2:18" ht="30" x14ac:dyDescent="0.25">
-      <c r="B46" s="6" t="s">
-        <v>22</v>
+      <c r="M45" s="4" t="s">
+        <v>110</v>
+      </c>
+      <c r="O45" t="s">
+        <v>24</v>
+      </c>
+      <c r="P45" t="s">
+        <v>312</v>
+      </c>
+      <c r="Q45" s="4" t="s">
+        <v>110</v>
+      </c>
+    </row>
+    <row r="46" spans="1:22" ht="30" x14ac:dyDescent="0.25">
+      <c r="A46" s="8" t="s">
+        <v>23</v>
+      </c>
+      <c r="B46" t="s">
+        <v>327</v>
       </c>
       <c r="C46" t="s">
-        <v>61</v>
+        <v>327</v>
       </c>
       <c r="D46" t="s">
-        <v>171</v>
-      </c>
-      <c r="E46" s="4" t="s">
+        <v>327</v>
+      </c>
+      <c r="F46" s="6" t="s">
+        <v>23</v>
+      </c>
+      <c r="G46" t="s">
+        <v>62</v>
+      </c>
+      <c r="H46" t="s">
+        <v>173</v>
+      </c>
+      <c r="I46" s="4" t="s">
+        <v>111</v>
+      </c>
+      <c r="K46" t="s">
+        <v>62</v>
+      </c>
+      <c r="L46" t="s">
+        <v>249</v>
+      </c>
+      <c r="M46" s="4" t="s">
+        <v>111</v>
+      </c>
+      <c r="O46" t="s">
+        <v>62</v>
+      </c>
+      <c r="P46" t="s">
+        <v>313</v>
+      </c>
+      <c r="Q46" s="4" t="s">
+        <v>111</v>
+      </c>
+    </row>
+    <row r="47" spans="1:22" ht="45" x14ac:dyDescent="0.25">
+      <c r="A47" s="8" t="s">
+        <v>23</v>
+      </c>
+      <c r="B47" t="s">
+        <v>327</v>
+      </c>
+      <c r="C47" t="s">
+        <v>327</v>
+      </c>
+      <c r="D47" t="s">
+        <v>327</v>
+      </c>
+      <c r="F47" s="6" t="s">
+        <v>23</v>
+      </c>
+      <c r="G47" t="s">
+        <v>63</v>
+      </c>
+      <c r="H47" t="s">
+        <v>174</v>
+      </c>
+      <c r="I47" s="4" t="s">
+        <v>112</v>
+      </c>
+      <c r="K47" t="s">
+        <v>63</v>
+      </c>
+      <c r="L47" t="s">
+        <v>250</v>
+      </c>
+      <c r="M47" s="4" t="s">
+        <v>112</v>
+      </c>
+      <c r="O47" t="s">
+        <v>63</v>
+      </c>
+      <c r="P47" t="s">
+        <v>314</v>
+      </c>
+      <c r="Q47" s="4" t="s">
+        <v>112</v>
+      </c>
+      <c r="U47" t="s">
+        <v>209</v>
+      </c>
+      <c r="V47" t="s">
         <v>215</v>
       </c>
-      <c r="G46" t="s">
-        <v>206</v>
-      </c>
-      <c r="H46" t="s">
-        <v>249</v>
-      </c>
-      <c r="I46" s="4" t="s">
-        <v>215</v>
-      </c>
-    </row>
-    <row r="47" spans="2:18" x14ac:dyDescent="0.25">
-      <c r="B47" s="6" t="s">
+    </row>
+    <row r="48" spans="1:22" ht="60" x14ac:dyDescent="0.25">
+      <c r="A48" s="8" t="s">
         <v>23</v>
       </c>
-      <c r="C47" t="s">
-        <v>24</v>
-      </c>
-      <c r="D47" t="s">
-        <v>172</v>
-      </c>
-      <c r="E47" s="4" t="s">
-        <v>110</v>
-      </c>
-      <c r="G47" t="s">
-        <v>24</v>
-      </c>
-      <c r="H47" t="s">
-        <v>250</v>
-      </c>
-      <c r="I47" s="4" t="s">
-        <v>110</v>
-      </c>
-    </row>
-    <row r="48" spans="2:18" x14ac:dyDescent="0.25">
-      <c r="B48" s="6" t="s">
+      <c r="B48" t="s">
+        <v>327</v>
+      </c>
+      <c r="C48" t="s">
+        <v>327</v>
+      </c>
+      <c r="D48" t="s">
+        <v>327</v>
+      </c>
+      <c r="F48" s="6" t="s">
         <v>23</v>
       </c>
-      <c r="C48" t="s">
-        <v>62</v>
-      </c>
-      <c r="D48" t="s">
-        <v>173</v>
-      </c>
-      <c r="E48" s="4" t="s">
-        <v>111</v>
-      </c>
       <c r="G48" t="s">
-        <v>62</v>
+        <v>64</v>
       </c>
       <c r="H48" t="s">
+        <v>175</v>
+      </c>
+      <c r="I48" s="4" t="s">
+        <v>113</v>
+      </c>
+      <c r="K48" t="s">
+        <v>64</v>
+      </c>
+      <c r="L48" t="s">
         <v>251</v>
       </c>
-      <c r="I48" s="4" t="s">
-        <v>111</v>
-      </c>
-    </row>
-    <row r="49" spans="2:18" ht="30" x14ac:dyDescent="0.25">
-      <c r="B49" s="6" t="s">
+      <c r="M48" s="4" t="s">
+        <v>113</v>
+      </c>
+      <c r="O48" t="s">
+        <v>64</v>
+      </c>
+      <c r="P48" t="s">
+        <v>315</v>
+      </c>
+      <c r="Q48" s="4" t="s">
+        <v>113</v>
+      </c>
+      <c r="U48" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="49" spans="1:17" ht="30" x14ac:dyDescent="0.25">
+      <c r="A49" s="8" t="s">
         <v>23</v>
       </c>
+      <c r="B49" t="s">
+        <v>327</v>
+      </c>
       <c r="C49" t="s">
-        <v>63</v>
+        <v>327</v>
       </c>
       <c r="D49" t="s">
-        <v>174</v>
-      </c>
-      <c r="E49" s="4" t="s">
-        <v>112</v>
+        <v>327</v>
+      </c>
+      <c r="F49" s="6" t="s">
+        <v>23</v>
       </c>
       <c r="G49" t="s">
-        <v>63</v>
+        <v>65</v>
       </c>
       <c r="H49" t="s">
+        <v>176</v>
+      </c>
+      <c r="I49" s="4" t="s">
+        <v>114</v>
+      </c>
+      <c r="K49" t="s">
+        <v>65</v>
+      </c>
+      <c r="L49" t="s">
         <v>252</v>
       </c>
-      <c r="I49" s="4" t="s">
-        <v>112</v>
-      </c>
-      <c r="Q49" t="s">
+      <c r="M49" s="4" t="s">
+        <v>114</v>
+      </c>
+      <c r="O49" t="s">
+        <v>65</v>
+      </c>
+      <c r="P49" t="s">
+        <v>316</v>
+      </c>
+      <c r="Q49" s="4" t="s">
+        <v>114</v>
+      </c>
+    </row>
+    <row r="50" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A50" s="8" t="s">
+        <v>25</v>
+      </c>
+      <c r="B50" t="s">
+        <v>327</v>
+      </c>
+      <c r="C50" t="s">
+        <v>327</v>
+      </c>
+      <c r="D50" t="s">
+        <v>327</v>
+      </c>
+      <c r="F50" s="6" t="s">
+        <v>25</v>
+      </c>
+      <c r="G50" t="s">
+        <v>117</v>
+      </c>
+      <c r="H50" t="s">
+        <v>177</v>
+      </c>
+      <c r="I50" s="4" t="s">
+        <v>116</v>
+      </c>
+      <c r="K50" t="s">
+        <v>117</v>
+      </c>
+      <c r="L50" t="s">
+        <v>253</v>
+      </c>
+      <c r="M50" s="4" t="s">
+        <v>116</v>
+      </c>
+      <c r="O50" t="s">
+        <v>117</v>
+      </c>
+      <c r="P50" t="s">
+        <v>317</v>
+      </c>
+      <c r="Q50" s="4" t="s">
+        <v>116</v>
+      </c>
+    </row>
+    <row r="51" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A51" s="8" t="s">
+        <v>25</v>
+      </c>
+      <c r="B51" t="s">
+        <v>327</v>
+      </c>
+      <c r="C51" t="s">
+        <v>327</v>
+      </c>
+      <c r="D51" t="s">
+        <v>327</v>
+      </c>
+      <c r="F51" s="6" t="s">
+        <v>25</v>
+      </c>
+      <c r="G51" t="s">
+        <v>118</v>
+      </c>
+      <c r="H51" t="s">
+        <v>178</v>
+      </c>
+      <c r="I51" s="4" t="s">
+        <v>121</v>
+      </c>
+      <c r="K51" t="s">
+        <v>118</v>
+      </c>
+      <c r="L51" t="s">
+        <v>254</v>
+      </c>
+      <c r="M51" s="4" t="s">
+        <v>121</v>
+      </c>
+      <c r="O51" t="s">
+        <v>118</v>
+      </c>
+      <c r="P51" t="s">
+        <v>318</v>
+      </c>
+      <c r="Q51" s="4" t="s">
+        <v>121</v>
+      </c>
+    </row>
+    <row r="52" spans="1:17" ht="30" x14ac:dyDescent="0.25">
+      <c r="A52" s="8" t="s">
+        <v>25</v>
+      </c>
+      <c r="B52" t="s">
+        <v>327</v>
+      </c>
+      <c r="C52" t="s">
+        <v>327</v>
+      </c>
+      <c r="D52" t="s">
+        <v>327</v>
+      </c>
+      <c r="F52" s="6" t="s">
+        <v>25</v>
+      </c>
+      <c r="G52" t="s">
+        <v>119</v>
+      </c>
+      <c r="H52" t="s">
+        <v>179</v>
+      </c>
+      <c r="I52" s="4" t="s">
+        <v>122</v>
+      </c>
+      <c r="K52" t="s">
+        <v>119</v>
+      </c>
+      <c r="L52" t="s">
+        <v>255</v>
+      </c>
+      <c r="M52" s="4" t="s">
+        <v>122</v>
+      </c>
+      <c r="O52" t="s">
+        <v>119</v>
+      </c>
+      <c r="P52" t="s">
+        <v>319</v>
+      </c>
+      <c r="Q52" s="4" t="s">
+        <v>122</v>
+      </c>
+    </row>
+    <row r="53" spans="1:17" ht="30" x14ac:dyDescent="0.25">
+      <c r="A53" s="8" t="s">
+        <v>25</v>
+      </c>
+      <c r="B53" t="s">
+        <v>327</v>
+      </c>
+      <c r="C53" t="s">
+        <v>327</v>
+      </c>
+      <c r="D53" t="s">
+        <v>327</v>
+      </c>
+      <c r="F53" s="6" t="s">
+        <v>25</v>
+      </c>
+      <c r="G53" t="s">
+        <v>120</v>
+      </c>
+      <c r="H53" t="s">
+        <v>180</v>
+      </c>
+      <c r="I53" s="4" t="s">
+        <v>123</v>
+      </c>
+      <c r="K53" t="s">
+        <v>120</v>
+      </c>
+      <c r="L53" t="s">
+        <v>256</v>
+      </c>
+      <c r="M53" s="4" t="s">
+        <v>123</v>
+      </c>
+      <c r="O53" t="s">
+        <v>120</v>
+      </c>
+      <c r="P53" t="s">
+        <v>320</v>
+      </c>
+      <c r="Q53" s="4" t="s">
+        <v>123</v>
+      </c>
+    </row>
+    <row r="54" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A54" s="8" t="s">
+        <v>126</v>
+      </c>
+      <c r="B54" t="s">
+        <v>327</v>
+      </c>
+      <c r="C54" t="s">
+        <v>327</v>
+      </c>
+      <c r="D54" t="s">
+        <v>327</v>
+      </c>
+      <c r="F54" s="6" t="s">
+        <v>126</v>
+      </c>
+      <c r="G54" t="s">
+        <v>68</v>
+      </c>
+      <c r="H54" t="s">
+        <v>181</v>
+      </c>
+      <c r="I54" s="4" t="s">
+        <v>124</v>
+      </c>
+      <c r="K54" t="s">
         <v>210</v>
       </c>
-      <c r="R49" t="s">
-        <v>217</v>
-      </c>
-    </row>
-    <row r="50" spans="2:18" ht="45" x14ac:dyDescent="0.25">
-      <c r="B50" s="6" t="s">
-        <v>23</v>
-      </c>
-      <c r="C50" t="s">
-        <v>64</v>
-      </c>
-      <c r="D50" t="s">
-        <v>175</v>
-      </c>
-      <c r="E50" s="4" t="s">
-        <v>113</v>
-      </c>
-      <c r="G50" t="s">
-        <v>64</v>
-      </c>
-      <c r="H50" t="s">
-        <v>253</v>
-      </c>
-      <c r="I50" s="4" t="s">
-        <v>113</v>
-      </c>
-      <c r="Q50" t="s">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="51" spans="2:18" x14ac:dyDescent="0.25">
-      <c r="B51" s="6" t="s">
-        <v>23</v>
-      </c>
-      <c r="C51" t="s">
-        <v>65</v>
-      </c>
-      <c r="D51" t="s">
-        <v>176</v>
-      </c>
-      <c r="E51" s="4" t="s">
-        <v>114</v>
-      </c>
-      <c r="G51" t="s">
-        <v>65</v>
-      </c>
-      <c r="H51" t="s">
-        <v>254</v>
-      </c>
-      <c r="I51" s="4" t="s">
-        <v>114</v>
-      </c>
-    </row>
-    <row r="52" spans="2:18" x14ac:dyDescent="0.25">
-      <c r="B52" s="6" t="s">
-        <v>25</v>
-      </c>
-      <c r="C52" t="s">
-        <v>117</v>
-      </c>
-      <c r="D52" t="s">
-        <v>177</v>
-      </c>
-      <c r="E52" s="4" t="s">
-        <v>116</v>
-      </c>
-      <c r="G52" t="s">
-        <v>117</v>
-      </c>
-      <c r="H52" t="s">
-        <v>255</v>
-      </c>
-      <c r="I52" s="4" t="s">
-        <v>116</v>
-      </c>
-    </row>
-    <row r="53" spans="2:18" x14ac:dyDescent="0.25">
-      <c r="B53" s="6" t="s">
-        <v>25</v>
-      </c>
-      <c r="C53" t="s">
-        <v>118</v>
-      </c>
-      <c r="D53" t="s">
-        <v>178</v>
-      </c>
-      <c r="E53" s="4" t="s">
-        <v>121</v>
-      </c>
-      <c r="G53" t="s">
-        <v>118</v>
-      </c>
-      <c r="H53" t="s">
-        <v>256</v>
-      </c>
-      <c r="I53" s="4" t="s">
-        <v>121</v>
-      </c>
-    </row>
-    <row r="54" spans="2:18" x14ac:dyDescent="0.25">
-      <c r="B54" s="6" t="s">
-        <v>25</v>
-      </c>
-      <c r="C54" t="s">
-        <v>119</v>
-      </c>
-      <c r="D54" t="s">
-        <v>179</v>
-      </c>
-      <c r="E54" s="4" t="s">
-        <v>122</v>
-      </c>
-      <c r="G54" t="s">
-        <v>119</v>
-      </c>
-      <c r="H54" t="s">
+      <c r="L54" t="s">
         <v>257</v>
       </c>
-      <c r="I54" s="4" t="s">
-        <v>122</v>
-      </c>
-    </row>
-    <row r="55" spans="2:18" x14ac:dyDescent="0.25">
-      <c r="B55" s="6" t="s">
-        <v>25</v>
+      <c r="M54" s="4" t="s">
+        <v>124</v>
+      </c>
+      <c r="O54" t="s">
+        <v>210</v>
+      </c>
+      <c r="P54" t="s">
+        <v>321</v>
+      </c>
+      <c r="Q54" s="4" t="s">
+        <v>124</v>
+      </c>
+    </row>
+    <row r="55" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A55" s="8" t="s">
+        <v>126</v>
+      </c>
+      <c r="B55" t="s">
+        <v>327</v>
       </c>
       <c r="C55" t="s">
-        <v>120</v>
+        <v>327</v>
       </c>
       <c r="D55" t="s">
-        <v>180</v>
-      </c>
-      <c r="E55" s="4" t="s">
-        <v>123</v>
+        <v>327</v>
+      </c>
+      <c r="F55" s="6" t="s">
+        <v>126</v>
       </c>
       <c r="G55" t="s">
-        <v>120</v>
+        <v>67</v>
       </c>
       <c r="H55" t="s">
+        <v>182</v>
+      </c>
+      <c r="I55" s="4" t="s">
+        <v>125</v>
+      </c>
+      <c r="K55" t="s">
+        <v>67</v>
+      </c>
+      <c r="L55" t="s">
         <v>258</v>
       </c>
-      <c r="I55" s="4" t="s">
-        <v>123</v>
-      </c>
-    </row>
-    <row r="56" spans="2:18" x14ac:dyDescent="0.25">
-      <c r="B56" s="6" t="s">
-        <v>126</v>
+      <c r="M55" s="4" t="s">
+        <v>125</v>
+      </c>
+      <c r="O55" t="s">
+        <v>67</v>
+      </c>
+      <c r="P55" t="s">
+        <v>322</v>
+      </c>
+      <c r="Q55" s="4" t="s">
+        <v>125</v>
+      </c>
+    </row>
+    <row r="56" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A56" s="8" t="s">
+        <v>127</v>
+      </c>
+      <c r="B56" t="s">
+        <v>327</v>
       </c>
       <c r="C56" t="s">
-        <v>68</v>
+        <v>327</v>
       </c>
       <c r="D56" t="s">
-        <v>181</v>
-      </c>
-      <c r="E56" s="4" t="s">
-        <v>124</v>
+        <v>327</v>
+      </c>
+      <c r="F56" s="6" t="s">
+        <v>127</v>
       </c>
       <c r="G56" t="s">
+        <v>26</v>
+      </c>
+      <c r="H56" t="s">
+        <v>183</v>
+      </c>
+      <c r="K56" t="s">
         <v>211</v>
       </c>
-      <c r="H56" t="s">
+      <c r="L56" t="s">
         <v>259</v>
       </c>
-      <c r="I56" s="4" t="s">
-        <v>124</v>
-      </c>
-    </row>
-    <row r="57" spans="2:18" x14ac:dyDescent="0.25">
-      <c r="B57" s="6" t="s">
-        <v>126</v>
+      <c r="O56" t="s">
+        <v>211</v>
+      </c>
+      <c r="P56" t="s">
+        <v>323</v>
+      </c>
+    </row>
+    <row r="57" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A57" s="8" t="s">
+        <v>127</v>
+      </c>
+      <c r="B57" t="s">
+        <v>327</v>
       </c>
       <c r="C57" t="s">
-        <v>67</v>
+        <v>327</v>
       </c>
       <c r="D57" t="s">
-        <v>182</v>
-      </c>
-      <c r="E57" s="4" t="s">
-        <v>125</v>
+        <v>327</v>
+      </c>
+      <c r="F57" s="6" t="s">
+        <v>127</v>
       </c>
       <c r="G57" t="s">
-        <v>67</v>
+        <v>27</v>
       </c>
       <c r="H57" t="s">
+        <v>184</v>
+      </c>
+      <c r="K57" t="s">
+        <v>212</v>
+      </c>
+      <c r="L57" t="s">
         <v>260</v>
       </c>
-      <c r="I57" s="4" t="s">
-        <v>125</v>
-      </c>
-    </row>
-    <row r="58" spans="2:18" x14ac:dyDescent="0.25">
-      <c r="B58" s="6" t="s">
-        <v>127</v>
+      <c r="O57" t="s">
+        <v>212</v>
+      </c>
+      <c r="P57" t="s">
+        <v>324</v>
+      </c>
+    </row>
+    <row r="58" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A58" s="8" t="s">
+        <v>128</v>
+      </c>
+      <c r="B58" t="s">
+        <v>327</v>
       </c>
       <c r="C58" t="s">
-        <v>26</v>
+        <v>327</v>
       </c>
       <c r="D58" t="s">
-        <v>183</v>
+        <v>327</v>
+      </c>
+      <c r="F58" s="6" t="s">
+        <v>128</v>
       </c>
       <c r="G58" t="s">
-        <v>212</v>
+        <v>28</v>
       </c>
       <c r="H58" t="s">
+        <v>185</v>
+      </c>
+      <c r="K58" t="s">
+        <v>189</v>
+      </c>
+      <c r="L58" t="s">
         <v>261</v>
       </c>
-    </row>
-    <row r="59" spans="2:18" x14ac:dyDescent="0.25">
-      <c r="B59" s="6" t="s">
-        <v>127</v>
-      </c>
-      <c r="C59" t="s">
-        <v>27</v>
-      </c>
-      <c r="D59" t="s">
-        <v>184</v>
+      <c r="O58" t="s">
+        <v>189</v>
+      </c>
+      <c r="P58" t="s">
+        <v>325</v>
+      </c>
+    </row>
+    <row r="59" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A59" s="6" t="s">
+        <v>128</v>
+      </c>
+      <c r="B59" t="s">
+        <v>327</v>
+      </c>
+      <c r="F59" s="6" t="s">
+        <v>128</v>
       </c>
       <c r="G59" t="s">
-        <v>213</v>
+        <v>29</v>
       </c>
       <c r="H59" t="s">
+        <v>186</v>
+      </c>
+    </row>
+    <row r="60" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A60" s="6" t="s">
+        <v>128</v>
+      </c>
+      <c r="B60" t="s">
+        <v>327</v>
+      </c>
+      <c r="F60" s="6" t="s">
+        <v>128</v>
+      </c>
+      <c r="G60" t="s">
+        <v>30</v>
+      </c>
+      <c r="H60" t="s">
+        <v>187</v>
+      </c>
+    </row>
+    <row r="61" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A61" s="8" t="s">
+        <v>128</v>
+      </c>
+      <c r="B61" t="s">
+        <v>327</v>
+      </c>
+      <c r="C61" t="s">
+        <v>327</v>
+      </c>
+      <c r="D61" t="s">
+        <v>327</v>
+      </c>
+      <c r="F61" s="6" t="s">
+        <v>128</v>
+      </c>
+      <c r="G61" t="s">
+        <v>31</v>
+      </c>
+      <c r="H61" t="s">
+        <v>188</v>
+      </c>
+      <c r="K61" t="s">
+        <v>31</v>
+      </c>
+      <c r="L61" t="s">
         <v>262</v>
       </c>
-    </row>
-    <row r="60" spans="2:18" x14ac:dyDescent="0.25">
-      <c r="B60" s="6" t="s">
-        <v>128</v>
-      </c>
-      <c r="C60" t="s">
-        <v>28</v>
-      </c>
-      <c r="D60" t="s">
-        <v>185</v>
-      </c>
-      <c r="G60" t="s">
-        <v>189</v>
-      </c>
-      <c r="H60" t="s">
-        <v>263</v>
-      </c>
-    </row>
-    <row r="61" spans="2:18" x14ac:dyDescent="0.25">
-      <c r="B61" t="s">
-        <v>128</v>
-      </c>
-      <c r="C61" t="s">
-        <v>29</v>
-      </c>
-      <c r="D61" t="s">
-        <v>186</v>
-      </c>
-    </row>
-    <row r="62" spans="2:18" x14ac:dyDescent="0.25">
-      <c r="B62" t="s">
-        <v>128</v>
-      </c>
-      <c r="C62" t="s">
-        <v>30</v>
-      </c>
-      <c r="D62" t="s">
-        <v>187</v>
-      </c>
-    </row>
-    <row r="63" spans="2:18" x14ac:dyDescent="0.25">
-      <c r="B63" s="6" t="s">
-        <v>128</v>
-      </c>
-      <c r="C63" t="s">
+      <c r="O61" t="s">
         <v>31</v>
       </c>
-      <c r="D63" t="s">
-        <v>188</v>
-      </c>
-      <c r="G63" t="s">
-        <v>31</v>
-      </c>
-      <c r="H63" t="s">
-        <v>264</v>
+      <c r="P61" t="s">
+        <v>326</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Data is ready for coding
1. CCES_Data_Cleaning_Final.ipynb:
This is the jupyter notebook I used to import the data, clean it, and write it to a sqlite file. The notebook has good notes throughout to explain all of the processes.

2. data_raw folder:
tab file with survey responses - this is the primary source of raw data.
csv file with state names and a common column V101 with the tab file.

3. db\CCES_Ver50.sqlite
This is the sqlite file that should be used for all queries.
There are example queries in the jupyter notebook to help with the class, column names, session.query syntax, etc.
</commit_message>
<xml_diff>
--- a/Variable_Index.xlsx
+++ b/Variable_Index.xlsx
@@ -8,14 +8,15 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\dkrei\Desktop\Coding_Bootcamp\DataBootCamp\CCES_Project2\CCES_Analysis_2016\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EAC453F5-B018-4A6B-83EF-CD52FB65042E}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A77283AC-CF4E-473B-9639-4004DFC59894}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="13800" windowHeight="4416" activeTab="2" xr2:uid="{B1787686-8DD4-4EAF-A6DB-220586B0E0A3}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="13800" windowHeight="4416" xr2:uid="{B1787686-8DD4-4EAF-A6DB-220586B0E0A3}"/>
   </bookViews>
   <sheets>
     <sheet name="3 Year Overview" sheetId="1" r:id="rId1"/>
     <sheet name="List of Variables" sheetId="2" r:id="rId2"/>
-    <sheet name="Section Questions" sheetId="3" r:id="rId3"/>
+    <sheet name="CCES_Ver1 Variables" sheetId="4" r:id="rId3"/>
+    <sheet name="Section Questions" sheetId="3" r:id="rId4"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -33,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="904" uniqueCount="344">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="948" uniqueCount="345">
   <si>
     <t>ID</t>
   </si>
@@ -1065,6 +1066,9 @@
   </si>
   <si>
     <t>Legal status for US HS Grads ('15, '16)</t>
+  </si>
+  <si>
+    <t>Prohibit MoreThan20 Weeks_16</t>
   </si>
 </sst>
 </file>
@@ -1478,8 +1482,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8B0C4685-FCD9-4520-9F28-50A98CF8260A}">
   <dimension ref="A1:V61"/>
   <sheetViews>
-    <sheetView topLeftCell="A34" workbookViewId="0">
-      <selection activeCell="I44" sqref="I44"/>
+    <sheetView tabSelected="1" topLeftCell="A34" workbookViewId="0">
+      <selection activeCell="H42" sqref="H42"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -2985,7 +2989,7 @@
         <v>57</v>
       </c>
       <c r="H40" t="s">
-        <v>167</v>
+        <v>344</v>
       </c>
       <c r="I40" s="4" t="s">
         <v>97</v>
@@ -3848,7 +3852,7 @@
   <dimension ref="A2:B61"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection sqref="A1:XFD1048576"/>
+      <selection activeCell="A22" sqref="A22:XFD22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -4343,11 +4347,206 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D2CA5A5D-B46E-49A1-90B2-73A9DCF9407F}">
+  <dimension ref="A2:B24"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="C3" sqref="C3"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="1" max="1" width="12.5546875" style="6" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="37.44140625" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="2" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A2" s="7" t="s">
+        <v>34</v>
+      </c>
+      <c r="B2" s="1" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A3" s="6" t="s">
+        <v>0</v>
+      </c>
+      <c r="B3" t="s">
+        <v>130</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A4" s="6" t="s">
+        <v>2</v>
+      </c>
+      <c r="B4" t="s">
+        <v>131</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A5" s="6" t="s">
+        <v>2</v>
+      </c>
+      <c r="B5" t="s">
+        <v>132</v>
+      </c>
+    </row>
+    <row r="6" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A6" s="6" t="s">
+        <v>2</v>
+      </c>
+      <c r="B6" t="s">
+        <v>133</v>
+      </c>
+    </row>
+    <row r="7" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A7" s="6" t="s">
+        <v>2</v>
+      </c>
+      <c r="B7" t="s">
+        <v>134</v>
+      </c>
+    </row>
+    <row r="8" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A8" s="6" t="s">
+        <v>7</v>
+      </c>
+      <c r="B8" t="s">
+        <v>135</v>
+      </c>
+    </row>
+    <row r="9" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A9" s="6" t="s">
+        <v>7</v>
+      </c>
+      <c r="B9" t="s">
+        <v>136</v>
+      </c>
+    </row>
+    <row r="10" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A10" s="6" t="s">
+        <v>7</v>
+      </c>
+      <c r="B10" t="s">
+        <v>137</v>
+      </c>
+    </row>
+    <row r="11" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A11" s="6" t="s">
+        <v>7</v>
+      </c>
+      <c r="B11" t="s">
+        <v>139</v>
+      </c>
+    </row>
+    <row r="12" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A12" s="6" t="s">
+        <v>13</v>
+      </c>
+      <c r="B12" t="s">
+        <v>140</v>
+      </c>
+    </row>
+    <row r="14" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A14" s="6" t="s">
+        <v>19</v>
+      </c>
+      <c r="B14" t="s">
+        <v>149</v>
+      </c>
+    </row>
+    <row r="15" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A15" s="6" t="s">
+        <v>19</v>
+      </c>
+      <c r="B15" t="s">
+        <v>150</v>
+      </c>
+    </row>
+    <row r="16" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A16" s="6" t="s">
+        <v>19</v>
+      </c>
+      <c r="B16" t="s">
+        <v>151</v>
+      </c>
+    </row>
+    <row r="17" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A17" s="6" t="s">
+        <v>19</v>
+      </c>
+      <c r="B17" t="s">
+        <v>152</v>
+      </c>
+    </row>
+    <row r="18" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A18" s="6" t="s">
+        <v>21</v>
+      </c>
+      <c r="B18" t="s">
+        <v>165</v>
+      </c>
+    </row>
+    <row r="19" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A19" s="6" t="s">
+        <v>21</v>
+      </c>
+      <c r="B19" t="s">
+        <v>166</v>
+      </c>
+    </row>
+    <row r="20" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A20" s="6" t="s">
+        <v>21</v>
+      </c>
+      <c r="B20" t="s">
+        <v>167</v>
+      </c>
+    </row>
+    <row r="21" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A21" s="6" t="s">
+        <v>21</v>
+      </c>
+      <c r="B21" t="s">
+        <v>168</v>
+      </c>
+    </row>
+    <row r="22" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A22" s="6" t="s">
+        <v>21</v>
+      </c>
+      <c r="B22" t="s">
+        <v>169</v>
+      </c>
+    </row>
+    <row r="23" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A23" s="6" t="s">
+        <v>21</v>
+      </c>
+      <c r="B23" t="s">
+        <v>170</v>
+      </c>
+    </row>
+    <row r="24" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A24" s="6" t="s">
+        <v>22</v>
+      </c>
+      <c r="B24" t="s">
+        <v>171</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C6535A0B-AD87-4C8A-AAB5-05F7E38C2C48}">
   <dimension ref="A2:C24"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C26" sqref="C26"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="K6" sqref="K6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>

</xml_diff>